<commit_message>
* All functions specific to master thesis deleted * Ready to be released as V3.0 * Updated graphics for github wiki * Updated readme * Includes results of test simulation
</commit_message>
<xml_diff>
--- a/inputs/test_input_template.xlsx
+++ b/inputs/test_input_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -1479,8 +1479,8 @@
   </sheetPr>
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16616,7 +16616,7 @@
   </sheetPr>
   <dimension ref="A1:AMD36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
* changed rectifiers -> inverters * edited fuel_consumption_kWh/fuel_consumption_l -> now the fuel consumption in results outputs is correct. Keep in mind: The optimization does NOT change with this patch, but only the display of results was misnamed. * terminal now also displays project_site_name in output at end of simulation * distributed files Z_* into the subsecquent modules using the functions. Now use should be more linear. If tool was integrated into wrapper: Keep in mind that files Z_* dont exist anymore, ie. intersections with your tool  might have to be adapted
</commit_message>
<xml_diff>
--- a/inputs/test_input_template.xlsx
+++ b/inputs/test_input_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="283">
   <si>
     <t xml:space="preserve">Tool for optimizing and simulating off- and on-grid electrification solutions</t>
   </si>
@@ -1479,8 +1479,8 @@
   </sheetPr>
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1666,7 +1666,7 @@
         <v>49</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1924,8 +1924,8 @@
   </sheetPr>
   <dimension ref="A1:G93"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B38" activeCellId="0" sqref="B38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A36" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A56" activeCellId="0" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2978,10 +2978,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3108,8 +3108,35 @@
         <v>208</v>
       </c>
     </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B11" s="20" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C11" s="20" t="n">
+        <v>1200</v>
+      </c>
+      <c r="D11" s="20" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="B12" s="20" t="n">
+        <v>15</v>
+      </c>
+      <c r="C12" s="20" t="n">
+        <v>25</v>
+      </c>
+      <c r="D12" s="20" t="n">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
-  <sheetProtection sheet="true" objects="true" scenarios="true"/>
   <mergeCells count="6">
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="B4:G4"/>
@@ -16616,8 +16643,8 @@
   </sheetPr>
   <dimension ref="A1:AMD36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -32003,7 +32030,7 @@
         <v>263</v>
       </c>
       <c r="B17" s="39" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C17" s="39" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
Add new parameters: "fuel_co2_emission_factor", "maingrid_co2_emission_factor"
</commit_message>
<xml_diff>
--- a/inputs/test_input_template.xlsx
+++ b/inputs/test_input_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="349">
   <si>
     <t xml:space="preserve">Tool for optimizing and simulating off- and on-grid electrification solutions</t>
   </si>
@@ -629,6 +629,18 @@
   </si>
   <si>
     <t xml:space="preserve">wind_lifetime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fuel_co2_emission_factor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kgCO2eq/l</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maingrid_co2_emission_factor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kgCO2eq/kWh</t>
   </si>
   <si>
     <t xml:space="preserve">Definition of sensitivity parameters</t>
@@ -1340,7 +1352,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="70">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1589,19 +1601,11 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1924,7 +1928,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="18.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.54"/>
@@ -2364,17 +2368,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G93"/>
+  <dimension ref="A1:G95"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A36" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A56" activeCellId="0" sqref="A56"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A75" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B96" activeCellId="0" sqref="B96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="6.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="24" width="6.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="24" width="6.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="4" style="0" width="8.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="6.09"/>
   </cols>
@@ -2767,7 +2771,7 @@
         <v>40</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>133</v>
+        <v>106</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3398,6 +3402,28 @@
       </c>
       <c r="C93" s="15" t="s">
         <v>106</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="B94" s="10" t="n">
+        <v>2.68</v>
+      </c>
+      <c r="C94" s="24" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="B95" s="10" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C95" s="24" t="s">
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -3428,7 +3454,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="20" width="12.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="20" width="12.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="20" width="9.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="20" width="6.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="8.54"/>
@@ -3438,7 +3464,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="15"/>
@@ -3454,10 +3480,10 @@
     </row>
     <row r="3" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="29" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -3483,7 +3509,7 @@
         <v>86</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="C5" s="32"/>
       <c r="D5" s="32"/>
@@ -3493,10 +3519,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="31" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -3506,10 +3532,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="31" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -3519,10 +3545,10 @@
     </row>
     <row r="8" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="31" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
@@ -3535,13 +3561,13 @@
         <v>86</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3612,15 +3638,15 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="20" width="8.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="20" width="9.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="10" style="20" width="6.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="20" width="12.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="20" width="11.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="20" width="12.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="20" width="11.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="21" style="20" width="6.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="6.91"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="I1" s="10"/>
       <c r="J1" s="15"/>
@@ -3631,10 +3657,10 @@
     </row>
     <row r="3" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="29" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -3647,10 +3673,10 @@
     </row>
     <row r="4" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="29" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
@@ -3663,10 +3689,10 @@
     </row>
     <row r="5" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="29" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
@@ -3679,10 +3705,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="12" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -3693,10 +3719,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="12" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -3707,10 +3733,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="12" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
@@ -3721,10 +3747,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
@@ -3735,10 +3761,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="12" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
@@ -3749,10 +3775,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="12" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -3763,10 +3789,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="12" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
@@ -3781,61 +3807,61 @@
     </row>
     <row r="14" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="20" t="s">
+        <v>236</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>222</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>224</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>237</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>238</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>230</v>
+      </c>
+      <c r="H14" s="20" t="s">
         <v>232</v>
       </c>
-      <c r="B14" s="20" t="s">
-        <v>218</v>
-      </c>
-      <c r="C14" s="20" t="s">
-        <v>220</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>233</v>
-      </c>
-      <c r="E14" s="20" t="s">
+      <c r="I14" s="20" t="s">
         <v>234</v>
-      </c>
-      <c r="F14" s="20" t="s">
-        <v>224</v>
-      </c>
-      <c r="G14" s="20" t="s">
-        <v>226</v>
-      </c>
-      <c r="H14" s="20" t="s">
-        <v>228</v>
-      </c>
-      <c r="I14" s="20" t="s">
-        <v>230</v>
       </c>
       <c r="L14" s="16"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="20" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="C15" s="20" t="s">
         <v>187</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="E15" s="20" t="s">
         <v>187</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="G15" s="20" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="H15" s="20" t="s">
         <v>187</v>
       </c>
       <c r="I15" s="20" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -3890,10 +3916,10 @@
     </row>
     <row r="3" customFormat="false" ht="23.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="29" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -3901,70 +3927,70 @@
     </row>
     <row r="4" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="35" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="C4" s="36"/>
       <c r="D4" s="36"/>
     </row>
     <row r="5" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="35" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="C5" s="36"/>
       <c r="D5" s="36"/>
     </row>
     <row r="6" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="35" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="C6" s="36"/>
       <c r="D6" s="36"/>
     </row>
     <row r="7" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="35" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="B7" s="35" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="C7" s="36"/>
       <c r="D7" s="36"/>
     </row>
     <row r="8" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="35" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="B8" s="35" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="C8" s="36"/>
       <c r="D8" s="36"/>
     </row>
     <row r="9" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="35" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="B9" s="35" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="C9" s="36"/>
       <c r="D9" s="36"/>
     </row>
     <row r="10" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="35" t="s">
+        <v>256</v>
+      </c>
+      <c r="B10" s="35" t="s">
         <v>252</v>
-      </c>
-      <c r="B10" s="35" t="s">
-        <v>248</v>
       </c>
       <c r="C10" s="36"/>
       <c r="D10" s="36"/>
@@ -3974,71 +4000,71 @@
         <v>43</v>
       </c>
       <c r="B11" s="35" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="C11" s="36"/>
       <c r="D11" s="36"/>
     </row>
     <row r="12" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="35" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="B12" s="35" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="C12" s="36"/>
       <c r="D12" s="36"/>
     </row>
     <row r="13" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="35" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="B13" s="35" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="C13" s="36"/>
       <c r="D13" s="36"/>
     </row>
     <row r="14" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="35" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="B14" s="35" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="C14" s="36"/>
       <c r="D14" s="36"/>
     </row>
     <row r="15" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="35" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="B15" s="35" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="C15" s="36"/>
       <c r="D15" s="36"/>
     </row>
     <row r="17" customFormat="false" ht="122.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="37" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="B17" s="38" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="C17" s="38" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="D17" s="38" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="E17" s="38" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="37" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="B18" s="39" t="s">
         <v>39</v>
@@ -4055,7 +4081,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="37" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="B19" s="39" t="s">
         <v>39</v>
@@ -4072,24 +4098,24 @@
     </row>
     <row r="20" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="37" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="B20" s="39" t="s">
         <v>187</v>
       </c>
       <c r="C20" s="39" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="D20" s="39" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="E20" s="39" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="37" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="B21" s="39" t="s">
         <v>187</v>
@@ -4101,12 +4127,12 @@
         <v>187</v>
       </c>
       <c r="E21" s="39" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="37" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="B22" s="39" t="s">
         <v>187</v>
@@ -4115,15 +4141,15 @@
         <v>187</v>
       </c>
       <c r="D22" s="39" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="E22" s="39" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="40" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="B23" s="39" t="s">
         <v>39</v>
@@ -4140,7 +4166,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="40" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="B24" s="39" t="s">
         <v>39</v>
@@ -4157,41 +4183,41 @@
     </row>
     <row r="25" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="37" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="B25" s="39" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="C25" s="39" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="D25" s="39" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="E25" s="39" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="37" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="B26" s="39" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="C26" s="39" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="D26" s="39" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="E26" s="39" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="40" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="B27" s="39" t="s">
         <v>39</v>
@@ -4208,24 +4234,24 @@
     </row>
     <row r="28" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="37" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="B28" s="39" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="C28" s="39" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="D28" s="39" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="E28" s="39" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="40" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="B29" s="39" t="s">
         <v>39</v>
@@ -4242,24 +4268,24 @@
     </row>
     <row r="30" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="40" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="B30" s="39" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="C30" s="39" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="D30" s="39" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="E30" s="39" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="37" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="B31" s="39" t="s">
         <v>187</v>
@@ -4276,7 +4302,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="37" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="B32" s="39" t="s">
         <v>187</v>
@@ -4310,41 +4336,41 @@
     </row>
     <row r="34" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="37" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="B34" s="39" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="C34" s="39" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="D34" s="39" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="E34" s="39" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="37" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="B35" s="39" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="C35" s="39" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="D35" s="39" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="E35" s="39" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="37" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="B36" s="39" t="s">
         <v>39</v>
@@ -4361,7 +4387,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="37" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="B37" s="39" t="s">
         <v>187</v>
@@ -4379,19 +4405,19 @@
     </row>
     <row r="38" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="37" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="B38" s="41" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="C38" s="41" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="D38" s="41" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="E38" s="41" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
     </row>
   </sheetData>
@@ -4415,13 +4441,13 @@
   </sheetPr>
   <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B43" activeCellId="0" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.54"/>
@@ -4434,7 +4460,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="42" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4442,10 +4468,10 @@
     </row>
     <row r="3" customFormat="false" ht="23.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="29" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -4456,10 +4482,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="35" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="B4" s="43" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="C4" s="43"/>
       <c r="D4" s="43"/>
@@ -4470,10 +4496,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="35" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="B5" s="43" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="C5" s="43"/>
       <c r="D5" s="43"/>
@@ -4484,10 +4510,10 @@
     </row>
     <row r="6" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="44" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -4498,10 +4524,10 @@
     </row>
     <row r="7" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="44" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="C7" s="30"/>
       <c r="D7" s="30"/>
@@ -4512,10 +4538,10 @@
     </row>
     <row r="8" customFormat="false" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="44" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="C8" s="30"/>
       <c r="D8" s="30"/>
@@ -4526,15 +4552,15 @@
     </row>
     <row r="10" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="45" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="B10" s="46" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="47" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="B11" s="47" t="n">
         <v>0.286229538687379</v>
@@ -4542,7 +4568,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="47" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="B12" s="47" t="n">
         <v>0.258073109045841</v>
@@ -4550,7 +4576,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="47" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="B13" s="47" t="n">
         <v>0.23396226376115</v>
@@ -4558,7 +4584,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="47" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="B14" s="47" t="n">
         <v>0.22173508850563</v>
@@ -4566,7 +4592,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E16" s="48" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="F16" s="48"/>
       <c r="G16" s="48"/>
@@ -4574,42 +4600,42 @@
     </row>
     <row r="17" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="49" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="B17" s="49" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="C17" s="50" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="D17" s="51" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="E17" s="48" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="F17" s="48" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="G17" s="48" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="H17" s="48" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="I17" s="48" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="52" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="B18" s="53" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="C18" s="54" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="D18" s="55" t="n">
         <v>0.513888888888889</v>
@@ -4619,16 +4645,16 @@
       <c r="G18" s="48"/>
       <c r="H18" s="48"/>
       <c r="I18" s="57" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="52"/>
       <c r="B19" s="58" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="C19" s="59" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="D19" s="60" t="n">
         <v>0.486111111111111</v>
@@ -4638,18 +4664,18 @@
       <c r="G19" s="48"/>
       <c r="H19" s="48"/>
       <c r="I19" s="57" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="52" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="B20" s="53" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="C20" s="54" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="D20" s="55" t="n">
         <v>0.259871031746032</v>
@@ -4659,18 +4685,18 @@
       <c r="G20" s="48"/>
       <c r="H20" s="48"/>
       <c r="I20" s="57" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="52"/>
       <c r="B21" s="61" t="s">
-        <v>321</v>
-      </c>
-      <c r="C21" s="62" t="s">
-        <v>322</v>
-      </c>
-      <c r="D21" s="63" t="n">
+        <v>325</v>
+      </c>
+      <c r="C21" s="47" t="s">
+        <v>326</v>
+      </c>
+      <c r="D21" s="62" t="n">
         <v>0.238492063492063</v>
       </c>
       <c r="E21" s="56"/>
@@ -4678,102 +4704,102 @@
       <c r="G21" s="48"/>
       <c r="H21" s="48"/>
       <c r="I21" s="57" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="52"/>
       <c r="B22" s="61" t="s">
-        <v>323</v>
-      </c>
-      <c r="C22" s="62" t="s">
-        <v>324</v>
-      </c>
-      <c r="D22" s="63" t="n">
+        <v>327</v>
+      </c>
+      <c r="C22" s="47" t="s">
+        <v>328</v>
+      </c>
+      <c r="D22" s="62" t="n">
         <v>0.246825396825397</v>
       </c>
-      <c r="E22" s="64" t="n">
+      <c r="E22" s="63" t="n">
         <v>2.75</v>
       </c>
-      <c r="F22" s="65" t="s">
+      <c r="F22" s="57" t="s">
         <v>187</v>
       </c>
-      <c r="G22" s="65" t="n">
+      <c r="G22" s="57" t="n">
         <v>1.88</v>
       </c>
-      <c r="H22" s="65" t="n">
+      <c r="H22" s="57" t="n">
         <v>3</v>
       </c>
       <c r="I22" s="57" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="52"/>
       <c r="B23" s="58" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="C23" s="59" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="D23" s="60" t="n">
         <v>0.254811507936508</v>
       </c>
-      <c r="E23" s="64" t="n">
+      <c r="E23" s="63" t="n">
         <v>2.25</v>
       </c>
-      <c r="F23" s="65" t="s">
+      <c r="F23" s="57" t="s">
         <v>187</v>
       </c>
-      <c r="G23" s="65" t="n">
+      <c r="G23" s="57" t="n">
         <v>1.5</v>
       </c>
-      <c r="H23" s="65" t="n">
+      <c r="H23" s="57" t="n">
         <v>3</v>
       </c>
       <c r="I23" s="57" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="66" t="s">
-        <v>327</v>
-      </c>
-      <c r="B24" s="67" t="s">
-        <v>328</v>
-      </c>
-      <c r="C24" s="62" t="s">
-        <v>329</v>
-      </c>
-      <c r="D24" s="63" t="n">
+      <c r="A24" s="64" t="s">
+        <v>331</v>
+      </c>
+      <c r="B24" s="65" t="s">
+        <v>332</v>
+      </c>
+      <c r="C24" s="47" t="s">
+        <v>333</v>
+      </c>
+      <c r="D24" s="62" t="n">
         <v>0.265354437229437</v>
       </c>
-      <c r="E24" s="64" t="n">
+      <c r="E24" s="63" t="n">
         <v>2</v>
       </c>
-      <c r="F24" s="65" t="s">
+      <c r="F24" s="57" t="s">
         <v>187</v>
       </c>
-      <c r="G24" s="65" t="n">
+      <c r="G24" s="57" t="n">
         <v>2.6</v>
       </c>
-      <c r="H24" s="65" t="n">
+      <c r="H24" s="57" t="n">
         <v>2.17</v>
       </c>
       <c r="I24" s="57" t="s">
-        <v>330</v>
-      </c>
-      <c r="N24" s="68"/>
+        <v>334</v>
+      </c>
+      <c r="N24" s="66"/>
     </row>
     <row r="25" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="66"/>
-      <c r="B25" s="67" t="s">
-        <v>331</v>
-      </c>
-      <c r="C25" s="62" t="s">
-        <v>332</v>
-      </c>
-      <c r="D25" s="63" t="n">
+      <c r="A25" s="64"/>
+      <c r="B25" s="65" t="s">
+        <v>335</v>
+      </c>
+      <c r="C25" s="47" t="s">
+        <v>336</v>
+      </c>
+      <c r="D25" s="62" t="n">
         <v>0.3964420995671</v>
       </c>
       <c r="E25" s="56"/>
@@ -4781,122 +4807,122 @@
       <c r="G25" s="48"/>
       <c r="H25" s="48"/>
       <c r="I25" s="57" t="s">
-        <v>315</v>
-      </c>
-      <c r="N25" s="68"/>
+        <v>319</v>
+      </c>
+      <c r="N25" s="66"/>
     </row>
     <row r="26" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="66"/>
-      <c r="B26" s="69" t="s">
-        <v>333</v>
+      <c r="A26" s="64"/>
+      <c r="B26" s="67" t="s">
+        <v>337</v>
       </c>
       <c r="C26" s="59" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="D26" s="60" t="n">
         <v>0.338203463203463</v>
       </c>
-      <c r="E26" s="64" t="n">
+      <c r="E26" s="63" t="n">
         <v>2.57</v>
       </c>
-      <c r="F26" s="65" t="s">
+      <c r="F26" s="57" t="s">
         <v>187</v>
       </c>
-      <c r="G26" s="65" t="n">
+      <c r="G26" s="57" t="n">
         <v>1.71</v>
       </c>
-      <c r="H26" s="65" t="n">
+      <c r="H26" s="57" t="n">
         <v>2.14</v>
       </c>
       <c r="I26" s="57" t="s">
-        <v>330</v>
-      </c>
-      <c r="N26" s="68"/>
+        <v>334</v>
+      </c>
+      <c r="N26" s="66"/>
     </row>
     <row r="27" customFormat="false" ht="12.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="70" t="s">
-        <v>335</v>
-      </c>
-      <c r="B27" s="71" t="s">
-        <v>336</v>
+      <c r="A27" s="68" t="s">
+        <v>339</v>
+      </c>
+      <c r="B27" s="69" t="s">
+        <v>340</v>
       </c>
       <c r="C27" s="54" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="D27" s="55" t="n">
         <v>0.255808080808081</v>
       </c>
-      <c r="E27" s="64" t="n">
+      <c r="E27" s="63" t="n">
         <v>0</v>
       </c>
-      <c r="F27" s="65" t="s">
+      <c r="F27" s="57" t="s">
         <v>187</v>
       </c>
-      <c r="G27" s="65" t="n">
+      <c r="G27" s="57" t="n">
         <v>0.77</v>
       </c>
-      <c r="H27" s="65" t="n">
+      <c r="H27" s="57" t="n">
         <v>0.44</v>
       </c>
       <c r="I27" s="57" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="J27" s="16" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="70"/>
-      <c r="B28" s="67" t="s">
-        <v>339</v>
-      </c>
-      <c r="C28" s="62" t="s">
-        <v>340</v>
-      </c>
-      <c r="D28" s="63" t="n">
+      <c r="A28" s="68"/>
+      <c r="B28" s="65" t="s">
+        <v>343</v>
+      </c>
+      <c r="C28" s="47" t="s">
+        <v>344</v>
+      </c>
+      <c r="D28" s="62" t="n">
         <v>0.383775252525253</v>
       </c>
-      <c r="E28" s="64" t="n">
+      <c r="E28" s="63" t="n">
         <v>2.63</v>
       </c>
-      <c r="F28" s="65" t="s">
+      <c r="F28" s="57" t="s">
         <v>187</v>
       </c>
-      <c r="G28" s="65" t="n">
+      <c r="G28" s="57" t="n">
         <v>1</v>
       </c>
-      <c r="H28" s="65" t="n">
+      <c r="H28" s="57" t="n">
         <v>1.88</v>
       </c>
       <c r="I28" s="57" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="70"/>
-      <c r="B29" s="69" t="s">
-        <v>341</v>
+      <c r="A29" s="68"/>
+      <c r="B29" s="67" t="s">
+        <v>345</v>
       </c>
       <c r="C29" s="59" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="D29" s="60" t="n">
         <v>0.360416666666667</v>
       </c>
-      <c r="E29" s="64" t="n">
+      <c r="E29" s="63" t="n">
         <v>1.63</v>
       </c>
-      <c r="F29" s="65" t="s">
+      <c r="F29" s="57" t="s">
         <v>187</v>
       </c>
-      <c r="G29" s="65" t="n">
+      <c r="G29" s="57" t="n">
         <v>1.5</v>
       </c>
-      <c r="H29" s="65" t="n">
+      <c r="H29" s="57" t="n">
         <v>2.63</v>
       </c>
       <c r="I29" s="57" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4908,16 +4934,16 @@
     </row>
     <row r="32" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="48" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="B32" s="48"/>
     </row>
     <row r="33" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="48" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="B33" s="48" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Update input file: output folder
</commit_message>
<xml_diff>
--- a/inputs/test_input_template.xlsx
+++ b/inputs/test_input_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="349">
   <si>
     <t>Tool for optimizing and simulating off- and on-grid electrification solutions</t>
   </si>
@@ -1104,12 +1104,6 @@
   </si>
   <si>
     <t>simulation_results</t>
-  </si>
-  <si>
-    <t>peak_demand</t>
-  </si>
-  <si>
-    <t>oem, string (name of base capacity case), None, peak_demand</t>
   </si>
 </sst>
 </file>
@@ -1420,6 +1414,39 @@
   </cellStyleXfs>
   <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1576,39 +1603,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1975,179 +1969,179 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
     </row>
     <row r="3" spans="2:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B3" s="1"/>
-      <c r="C3" s="2" t="s">
+      <c r="B3" s="12"/>
+      <c r="C3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
     </row>
     <row r="4" spans="2:6" ht="13" x14ac:dyDescent="0.3">
-      <c r="B4" s="1"/>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="12"/>
+      <c r="C4" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="1"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
     </row>
     <row r="6" spans="2:6" ht="23.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6" s="62" t="s">
+      <c r="B6" s="12"/>
+      <c r="C6" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="62"/>
-      <c r="E6" s="62"/>
-      <c r="F6" s="1"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="12"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="1" t="s">
+      <c r="B7" s="12"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="1"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="1" t="s">
+      <c r="B8" s="12"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="1"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="1" t="s">
+      <c r="B9" s="12"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="1"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="1" t="s">
+      <c r="B10" s="12"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="1"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="1" t="s">
+      <c r="B11" s="12"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="1"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="1" t="s">
+      <c r="B12" s="12"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="1"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
     </row>
     <row r="14" spans="2:6" ht="13" x14ac:dyDescent="0.3">
-      <c r="B14" s="1"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="5" t="s">
+      <c r="B14" s="12"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="1"/>
+      <c r="F14" s="12"/>
     </row>
     <row r="15" spans="2:6" ht="13" x14ac:dyDescent="0.25">
-      <c r="B15" s="1"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="6" t="s">
+      <c r="B15" s="12"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="1"/>
+      <c r="F15" s="12"/>
     </row>
     <row r="16" spans="2:6" ht="25" x14ac:dyDescent="0.25">
-      <c r="B16" s="1"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="6" t="s">
+      <c r="B16" s="12"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="F16" s="1"/>
+      <c r="F16" s="12"/>
     </row>
     <row r="17" spans="2:6" ht="13" x14ac:dyDescent="0.25">
-      <c r="B17" s="1"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="6" t="s">
+      <c r="B17" s="12"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="F17" s="1"/>
+      <c r="F17" s="12"/>
     </row>
     <row r="18" spans="2:6" ht="13" x14ac:dyDescent="0.25">
-      <c r="B18" s="1"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="6" t="s">
+      <c r="B18" s="12"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="F18" s="1"/>
+      <c r="F18" s="12"/>
     </row>
     <row r="19" spans="2:6" ht="13" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="6" t="s">
+      <c r="B19" s="12"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="F19" s="1"/>
+      <c r="F19" s="12"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
@@ -2167,121 +2161,121 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.08984375" customWidth="1"/>
     <col min="2" max="2" width="33.36328125" customWidth="1"/>
-    <col min="3" max="3" width="18.6328125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="18.6328125" style="20" customWidth="1"/>
     <col min="4" max="1025" width="8.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="21" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="13" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="63" t="s">
+      <c r="C3" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
     </row>
     <row r="4" spans="1:6" ht="13" x14ac:dyDescent="0.25">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="63" t="s">
+      <c r="C4" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
-      <c r="F4" s="63"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
     </row>
     <row r="5" spans="1:6" ht="13" x14ac:dyDescent="0.3">
-      <c r="A5" s="10"/>
-      <c r="B5" s="11" t="s">
+      <c r="A5" s="21"/>
+      <c r="B5" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="63" t="s">
+      <c r="C5" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
     </row>
     <row r="6" spans="1:6" ht="13" x14ac:dyDescent="0.3">
-      <c r="A6" s="10"/>
-      <c r="B6" s="11" t="s">
+      <c r="A6" s="21"/>
+      <c r="B6" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="63" t="s">
+      <c r="C6" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
     </row>
     <row r="7" spans="1:6" ht="13" x14ac:dyDescent="0.3">
-      <c r="A7" s="10"/>
-      <c r="B7" s="11" t="s">
+      <c r="A7" s="21"/>
+      <c r="B7" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="63" t="s">
+      <c r="C7" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="63"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="63"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
     </row>
     <row r="8" spans="1:6" ht="13" x14ac:dyDescent="0.3">
-      <c r="A8" s="10"/>
-      <c r="B8" s="11" t="s">
+      <c r="A8" s="21"/>
+      <c r="B8" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="63" t="s">
+      <c r="C8" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="63"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="63"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
     </row>
     <row r="9" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="10"/>
-      <c r="B9" s="11" t="s">
+      <c r="A9" s="21"/>
+      <c r="B9" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="64" t="s">
+      <c r="C9" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="64"/>
-      <c r="E9" s="64"/>
-      <c r="F9" s="64"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
     </row>
     <row r="10" spans="1:6" ht="13" x14ac:dyDescent="0.3">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="13"/>
+      <c r="A10" s="21"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="24"/>
     </row>
     <row r="11" spans="1:6" ht="13" x14ac:dyDescent="0.3">
-      <c r="A11" s="10"/>
-      <c r="B11" s="14" t="s">
+      <c r="A11" s="21"/>
+      <c r="B11" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="24" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="13" x14ac:dyDescent="0.3">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="21" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2289,7 +2283,7 @@
       <c r="B13" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="26" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2297,15 +2291,15 @@
       <c r="B14" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="15" t="s">
-        <v>39</v>
+      <c r="C14" s="26" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="26" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2313,7 +2307,7 @@
       <c r="B16" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="26" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2321,7 +2315,7 @@
       <c r="B17" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="16">
+      <c r="C17" s="27">
         <v>7</v>
       </c>
     </row>
@@ -2329,7 +2323,7 @@
       <c r="B18" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="17">
+      <c r="C18" s="28">
         <v>43101</v>
       </c>
     </row>
@@ -2337,7 +2331,7 @@
       <c r="B19" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="20" t="s">
         <v>47</v>
       </c>
       <c r="D19" t="s">
@@ -2348,7 +2342,7 @@
       <c r="B20" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="26" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2356,24 +2350,24 @@
       <c r="B21" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="26" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C22" s="18"/>
+      <c r="C22" s="29"/>
     </row>
     <row r="23" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="18"/>
+      <c r="C23" s="29"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="C24" s="27" t="s">
         <v>52</v>
       </c>
     </row>
@@ -2381,7 +2375,7 @@
       <c r="B25" t="s">
         <v>53</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="C25" s="26" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2389,7 +2383,7 @@
       <c r="B26" t="s">
         <v>54</v>
       </c>
-      <c r="C26" s="16" t="s">
+      <c r="C26" s="27" t="s">
         <v>55</v>
       </c>
       <c r="D26" t="s">
@@ -2400,25 +2394,25 @@
       <c r="B27" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="16">
+      <c r="C27" s="27">
         <v>0.03</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C28" s="18"/>
+      <c r="C28" s="29"/>
     </row>
     <row r="29" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="19"/>
+      <c r="C29" s="30"/>
     </row>
     <row r="30" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="10"/>
+      <c r="A30" s="21"/>
       <c r="B30" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="20" t="s">
+      <c r="C30" s="31" t="s">
         <v>59</v>
       </c>
       <c r="D30" t="s">
@@ -2426,39 +2420,39 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A31" s="10"/>
+      <c r="A31" s="21"/>
       <c r="B31" t="s">
         <v>61</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C31" s="20" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A32" s="10"/>
+      <c r="A32" s="21"/>
       <c r="B32" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="16" t="s">
+      <c r="C32" s="27" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C33" s="19"/>
+      <c r="C33" s="30"/>
     </row>
     <row r="34" spans="1:7" ht="13" x14ac:dyDescent="0.3">
-      <c r="A34" s="10" t="s">
+      <c r="A34" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="21"/>
-      <c r="G34" s="21"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="32"/>
+      <c r="G34" s="32"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>65</v>
       </c>
-      <c r="C35" s="15" t="s">
+      <c r="C35" s="26" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2466,8 +2460,8 @@
       <c r="B36" t="s">
         <v>66</v>
       </c>
-      <c r="C36" s="15" t="s">
-        <v>41</v>
+      <c r="C36" s="26" t="s">
+        <v>39</v>
       </c>
       <c r="D36" t="s">
         <v>67</v>
@@ -2477,7 +2471,7 @@
       <c r="B37" t="s">
         <v>68</v>
       </c>
-      <c r="C37" s="15" t="s">
+      <c r="C37" s="26" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2485,7 +2479,7 @@
       <c r="B38" t="s">
         <v>69</v>
       </c>
-      <c r="C38" s="15" t="s">
+      <c r="C38" s="26" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2493,7 +2487,7 @@
       <c r="B39" t="s">
         <v>70</v>
       </c>
-      <c r="C39" s="15" t="s">
+      <c r="C39" s="26" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2501,7 +2495,7 @@
       <c r="B40" t="s">
         <v>71</v>
       </c>
-      <c r="C40" s="15" t="s">
+      <c r="C40" s="26" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2509,25 +2503,25 @@
       <c r="B41" t="s">
         <v>72</v>
       </c>
-      <c r="C41" s="15" t="s">
+      <c r="C41" s="26" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C42" s="19"/>
+      <c r="C42" s="30"/>
     </row>
     <row r="43" spans="1:7" ht="13" x14ac:dyDescent="0.3">
-      <c r="A43" s="10" t="s">
+      <c r="A43" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="B43" s="10"/>
-      <c r="C43" s="19"/>
+      <c r="B43" s="21"/>
+      <c r="C43" s="30"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>73</v>
       </c>
-      <c r="C44" s="15" t="s">
+      <c r="C44" s="26" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2535,7 +2529,7 @@
       <c r="B45" t="s">
         <v>74</v>
       </c>
-      <c r="C45" s="15" t="s">
+      <c r="C45" s="26" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2543,24 +2537,24 @@
       <c r="B46" t="s">
         <v>75</v>
       </c>
-      <c r="C46" s="15" t="s">
+      <c r="C46" s="26" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C47" s="19"/>
+      <c r="C47" s="30"/>
     </row>
     <row r="48" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="10" t="s">
+      <c r="A48" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C48" s="18"/>
+      <c r="C48" s="29"/>
     </row>
     <row r="49" spans="2:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>76</v>
       </c>
-      <c r="C49" s="15" t="s">
+      <c r="C49" s="26" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2568,7 +2562,7 @@
       <c r="B50" t="s">
         <v>77</v>
       </c>
-      <c r="C50" s="15" t="s">
+      <c r="C50" s="26" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2576,7 +2570,7 @@
       <c r="B51" t="s">
         <v>78</v>
       </c>
-      <c r="C51" s="15" t="s">
+      <c r="C51" s="26" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2584,7 +2578,7 @@
       <c r="B52" t="s">
         <v>79</v>
       </c>
-      <c r="C52" s="15" t="s">
+      <c r="C52" s="26" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2611,74 +2605,74 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G95"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C94" sqref="C94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.81640625" customWidth="1"/>
-    <col min="2" max="2" width="6.08984375" style="9" customWidth="1"/>
-    <col min="3" max="3" width="6.6328125" style="22" customWidth="1"/>
+    <col min="2" max="2" width="6.08984375" style="20" customWidth="1"/>
+    <col min="3" max="3" width="6.6328125" style="33" customWidth="1"/>
     <col min="4" max="1023" width="8.6328125" customWidth="1"/>
     <col min="1024" max="1025" width="6.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
     </row>
     <row r="2" spans="1:7" ht="13" x14ac:dyDescent="0.3">
-      <c r="A2" s="10"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
     </row>
     <row r="3" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
     </row>
     <row r="4" spans="1:7" ht="46.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="64" t="s">
+      <c r="B4" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64"/>
-      <c r="G4" s="64"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
     </row>
     <row r="5" spans="1:7" ht="13" x14ac:dyDescent="0.3">
-      <c r="A5" s="10"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="25"/>
+      <c r="A5" s="21"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="36"/>
     </row>
     <row r="6" spans="1:7" ht="13" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="36" t="s">
         <v>87</v>
       </c>
     </row>
@@ -2686,10 +2680,10 @@
       <c r="A7" t="s">
         <v>88</v>
       </c>
-      <c r="B7" s="16">
+      <c r="B7" s="27">
         <v>0</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="24" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2697,10 +2691,10 @@
       <c r="A8" t="s">
         <v>90</v>
       </c>
-      <c r="B8" s="16">
+      <c r="B8" s="27">
         <v>0</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="24" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2708,10 +2702,10 @@
       <c r="A9" t="s">
         <v>92</v>
       </c>
-      <c r="B9" s="16">
+      <c r="B9" s="27">
         <v>0</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="24" t="s">
         <v>93</v>
       </c>
     </row>
@@ -2719,10 +2713,10 @@
       <c r="A10" t="s">
         <v>94</v>
       </c>
-      <c r="B10" s="16">
+      <c r="B10" s="27">
         <v>0</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="24" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2730,10 +2724,10 @@
       <c r="A11" t="s">
         <v>95</v>
       </c>
-      <c r="B11" s="16">
+      <c r="B11" s="27">
         <v>9.8000000000000007</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="24" t="s">
         <v>96</v>
       </c>
     </row>
@@ -2741,10 +2735,10 @@
       <c r="A12" t="s">
         <v>97</v>
       </c>
-      <c r="B12" s="16">
+      <c r="B12" s="27">
         <v>1</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="33" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2752,10 +2746,10 @@
       <c r="A13" t="s">
         <v>99</v>
       </c>
-      <c r="B13" s="16">
+      <c r="B13" s="27">
         <v>1</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="33" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2763,10 +2757,10 @@
       <c r="A14" t="s">
         <v>100</v>
       </c>
-      <c r="B14" s="16">
+      <c r="B14" s="27">
         <v>0</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="24" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2774,10 +2768,10 @@
       <c r="A15" t="s">
         <v>102</v>
       </c>
-      <c r="B15" s="16">
+      <c r="B15" s="27">
         <v>0</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="24" t="s">
         <v>103</v>
       </c>
     </row>
@@ -2785,10 +2779,10 @@
       <c r="A16" t="s">
         <v>104</v>
       </c>
-      <c r="B16" s="16">
+      <c r="B16" s="27">
         <v>40</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="24" t="s">
         <v>105</v>
       </c>
     </row>
@@ -2796,10 +2790,10 @@
       <c r="A17" t="s">
         <v>106</v>
       </c>
-      <c r="B17" s="16">
+      <c r="B17" s="27">
         <v>0.5</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="24" t="s">
         <v>107</v>
       </c>
     </row>
@@ -2807,10 +2801,10 @@
       <c r="A18" t="s">
         <v>108</v>
       </c>
-      <c r="B18" s="16">
+      <c r="B18" s="27">
         <v>820</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="24" t="s">
         <v>109</v>
       </c>
     </row>
@@ -2818,10 +2812,10 @@
       <c r="A19" t="s">
         <v>110</v>
       </c>
-      <c r="B19" s="16">
+      <c r="B19" s="27">
         <v>0.05</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="24" t="s">
         <v>111</v>
       </c>
     </row>
@@ -2829,10 +2823,10 @@
       <c r="A20" t="s">
         <v>112</v>
       </c>
-      <c r="B20" s="16">
+      <c r="B20" s="27">
         <v>0</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="24" t="s">
         <v>113</v>
       </c>
     </row>
@@ -2840,10 +2834,10 @@
       <c r="A21" t="s">
         <v>114</v>
       </c>
-      <c r="B21" s="16">
+      <c r="B21" s="27">
         <v>0.33</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="24" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2851,10 +2845,10 @@
       <c r="A22" t="s">
         <v>115</v>
       </c>
-      <c r="B22" s="16">
+      <c r="B22" s="27">
         <v>10</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="24" t="s">
         <v>105</v>
       </c>
     </row>
@@ -2862,10 +2856,10 @@
       <c r="A23" t="s">
         <v>116</v>
       </c>
-      <c r="B23" s="16">
+      <c r="B23" s="27">
         <v>1</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="24" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2873,10 +2867,10 @@
       <c r="A24" t="s">
         <v>117</v>
       </c>
-      <c r="B24" s="16">
+      <c r="B24" s="27">
         <v>0.1</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="24" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2884,10 +2878,10 @@
       <c r="A25" t="s">
         <v>118</v>
       </c>
-      <c r="B25" s="16">
+      <c r="B25" s="27">
         <v>1</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="24" t="s">
         <v>98</v>
       </c>
       <c r="D25" t="s">
@@ -2898,10 +2892,10 @@
       <c r="A26" t="s">
         <v>120</v>
       </c>
-      <c r="B26" s="16">
+      <c r="B26" s="27">
         <v>0.5</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="24" t="s">
         <v>107</v>
       </c>
     </row>
@@ -2909,10 +2903,10 @@
       <c r="A27" t="s">
         <v>121</v>
       </c>
-      <c r="B27" s="16">
+      <c r="B27" s="27">
         <v>0</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="24" t="s">
         <v>109</v>
       </c>
     </row>
@@ -2920,10 +2914,10 @@
       <c r="A28" t="s">
         <v>122</v>
       </c>
-      <c r="B28" s="16">
+      <c r="B28" s="27">
         <v>0</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="24" t="s">
         <v>111</v>
       </c>
     </row>
@@ -2931,10 +2925,10 @@
       <c r="A29" t="s">
         <v>123</v>
       </c>
-      <c r="B29" s="16">
+      <c r="B29" s="27">
         <v>0</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="24" t="s">
         <v>113</v>
       </c>
     </row>
@@ -2942,10 +2936,10 @@
       <c r="A30" t="s">
         <v>124</v>
       </c>
-      <c r="B30" s="9">
+      <c r="B30" s="20">
         <v>1</v>
       </c>
-      <c r="C30" s="22" t="s">
+      <c r="C30" s="33" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2953,10 +2947,10 @@
       <c r="A31" t="s">
         <v>125</v>
       </c>
-      <c r="B31" s="9">
+      <c r="B31" s="20">
         <v>15</v>
       </c>
-      <c r="C31" s="22" t="s">
+      <c r="C31" s="33" t="s">
         <v>105</v>
       </c>
     </row>
@@ -2964,10 +2958,10 @@
       <c r="A32" t="s">
         <v>126</v>
       </c>
-      <c r="B32" s="16">
+      <c r="B32" s="27">
         <v>1</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="24" t="s">
         <v>127</v>
       </c>
     </row>
@@ -2975,10 +2969,10 @@
       <c r="A33" t="s">
         <v>128</v>
       </c>
-      <c r="B33" s="16">
+      <c r="B33" s="27">
         <v>0.08</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="24" t="s">
         <v>113</v>
       </c>
     </row>
@@ -2986,10 +2980,10 @@
       <c r="A34" t="s">
         <v>129</v>
       </c>
-      <c r="B34" s="16">
+      <c r="B34" s="27">
         <v>0</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="C34" s="24" t="s">
         <v>130</v>
       </c>
     </row>
@@ -2997,10 +2991,10 @@
       <c r="A35" t="s">
         <v>131</v>
       </c>
-      <c r="B35" s="16">
+      <c r="B35" s="27">
         <v>0</v>
       </c>
-      <c r="C35" s="13" t="s">
+      <c r="C35" s="24" t="s">
         <v>132</v>
       </c>
     </row>
@@ -3008,10 +3002,10 @@
       <c r="A36" t="s">
         <v>133</v>
       </c>
-      <c r="B36" s="16">
+      <c r="B36" s="27">
         <v>40</v>
       </c>
-      <c r="C36" s="13" t="s">
+      <c r="C36" s="24" t="s">
         <v>105</v>
       </c>
     </row>
@@ -3019,10 +3013,10 @@
       <c r="A37" t="s">
         <v>134</v>
       </c>
-      <c r="B37" s="16">
+      <c r="B37" s="27">
         <v>0.05</v>
       </c>
-      <c r="C37" s="13" t="s">
+      <c r="C37" s="24" t="s">
         <v>113</v>
       </c>
     </row>
@@ -3030,10 +3024,10 @@
       <c r="A38" t="s">
         <v>135</v>
       </c>
-      <c r="B38" s="16">
+      <c r="B38" s="27">
         <v>0</v>
       </c>
-      <c r="C38" s="13" t="s">
+      <c r="C38" s="24" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3041,10 +3035,10 @@
       <c r="A39" t="s">
         <v>136</v>
       </c>
-      <c r="B39" s="16">
+      <c r="B39" s="27">
         <v>0</v>
       </c>
-      <c r="C39" s="13" t="s">
+      <c r="C39" s="24" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3052,10 +3046,10 @@
       <c r="A40" t="s">
         <v>137</v>
       </c>
-      <c r="B40" s="16">
+      <c r="B40" s="27">
         <v>1</v>
       </c>
-      <c r="C40" s="13" t="s">
+      <c r="C40" s="24" t="s">
         <v>107</v>
       </c>
     </row>
@@ -3063,10 +3057,10 @@
       <c r="A41" t="s">
         <v>138</v>
       </c>
-      <c r="B41" s="16">
+      <c r="B41" s="27">
         <v>200</v>
       </c>
-      <c r="C41" s="13" t="s">
+      <c r="C41" s="24" t="s">
         <v>109</v>
       </c>
     </row>
@@ -3074,10 +3068,10 @@
       <c r="A42" t="s">
         <v>139</v>
       </c>
-      <c r="B42" s="16">
+      <c r="B42" s="27">
         <v>0</v>
       </c>
-      <c r="C42" s="13" t="s">
+      <c r="C42" s="24" t="s">
         <v>111</v>
       </c>
     </row>
@@ -3085,10 +3079,10 @@
       <c r="A43" t="s">
         <v>140</v>
       </c>
-      <c r="B43" s="16">
+      <c r="B43" s="27">
         <v>0</v>
       </c>
-      <c r="C43" s="13" t="s">
+      <c r="C43" s="24" t="s">
         <v>113</v>
       </c>
     </row>
@@ -3096,10 +3090,10 @@
       <c r="A44" t="s">
         <v>141</v>
       </c>
-      <c r="B44" s="16">
+      <c r="B44" s="27">
         <v>1</v>
       </c>
-      <c r="C44" s="13" t="s">
+      <c r="C44" s="24" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3107,10 +3101,10 @@
       <c r="A45" t="s">
         <v>142</v>
       </c>
-      <c r="B45" s="16">
+      <c r="B45" s="27">
         <v>20</v>
       </c>
-      <c r="C45" s="13" t="s">
+      <c r="C45" s="24" t="s">
         <v>105</v>
       </c>
     </row>
@@ -3118,10 +3112,10 @@
       <c r="A46" t="s">
         <v>143</v>
       </c>
-      <c r="B46" s="16">
+      <c r="B46" s="27">
         <v>1.5</v>
       </c>
-      <c r="C46" s="13" t="s">
+      <c r="C46" s="24" t="s">
         <v>98</v>
       </c>
       <c r="D46" t="s">
@@ -3132,10 +3126,10 @@
       <c r="A47" t="s">
         <v>144</v>
       </c>
-      <c r="B47" s="16">
+      <c r="B47" s="27">
         <v>0.68</v>
       </c>
-      <c r="C47" s="13" t="s">
+      <c r="C47" s="24" t="s">
         <v>145</v>
       </c>
     </row>
@@ -3143,10 +3137,10 @@
       <c r="A48" t="s">
         <v>146</v>
       </c>
-      <c r="B48" s="16">
+      <c r="B48" s="27">
         <v>0.05</v>
       </c>
-      <c r="C48" s="13" t="s">
+      <c r="C48" s="24" t="s">
         <v>147</v>
       </c>
     </row>
@@ -3154,10 +3148,10 @@
       <c r="A49" t="s">
         <v>148</v>
       </c>
-      <c r="B49" s="16">
+      <c r="B49" s="27">
         <v>20000</v>
       </c>
-      <c r="C49" s="13" t="s">
+      <c r="C49" s="24" t="s">
         <v>101</v>
       </c>
     </row>
@@ -3165,10 +3159,10 @@
       <c r="A50" t="s">
         <v>149</v>
       </c>
-      <c r="B50" s="16">
+      <c r="B50" s="27">
         <v>0</v>
       </c>
-      <c r="C50" s="13" t="s">
+      <c r="C50" s="24" t="s">
         <v>103</v>
       </c>
     </row>
@@ -3176,10 +3170,10 @@
       <c r="A51" t="s">
         <v>150</v>
       </c>
-      <c r="B51" s="16">
+      <c r="B51" s="27">
         <v>20</v>
       </c>
-      <c r="C51" s="13" t="s">
+      <c r="C51" s="24" t="s">
         <v>105</v>
       </c>
     </row>
@@ -3187,10 +3181,10 @@
       <c r="A52" t="s">
         <v>151</v>
       </c>
-      <c r="B52" s="16">
+      <c r="B52" s="27">
         <v>0.5</v>
       </c>
-      <c r="C52" s="13" t="s">
+      <c r="C52" s="24" t="s">
         <v>152</v>
       </c>
     </row>
@@ -3198,10 +3192,10 @@
       <c r="A53" t="s">
         <v>153</v>
       </c>
-      <c r="B53" s="16">
+      <c r="B53" s="27">
         <v>1250</v>
       </c>
-      <c r="C53" s="13" t="s">
+      <c r="C53" s="24" t="s">
         <v>154</v>
       </c>
     </row>
@@ -3209,10 +3203,10 @@
       <c r="A54" t="s">
         <v>155</v>
       </c>
-      <c r="B54" s="16">
+      <c r="B54" s="27">
         <v>25</v>
       </c>
-      <c r="C54" s="13" t="s">
+      <c r="C54" s="24" t="s">
         <v>156</v>
       </c>
     </row>
@@ -3220,10 +3214,10 @@
       <c r="A55" t="s">
         <v>157</v>
       </c>
-      <c r="B55" s="16">
+      <c r="B55" s="27">
         <v>0</v>
       </c>
-      <c r="C55" s="13" t="s">
+      <c r="C55" s="24" t="s">
         <v>113</v>
       </c>
     </row>
@@ -3231,10 +3225,10 @@
       <c r="A56" t="s">
         <v>158</v>
       </c>
-      <c r="B56" s="16">
+      <c r="B56" s="27">
         <v>25</v>
       </c>
-      <c r="C56" s="13" t="s">
+      <c r="C56" s="24" t="s">
         <v>105</v>
       </c>
     </row>
@@ -3242,10 +3236,10 @@
       <c r="A57" t="s">
         <v>159</v>
       </c>
-      <c r="B57" s="16">
+      <c r="B57" s="27">
         <v>0.5</v>
       </c>
-      <c r="C57" s="13" t="s">
+      <c r="C57" s="24" t="s">
         <v>107</v>
       </c>
     </row>
@@ -3253,10 +3247,10 @@
       <c r="A58" t="s">
         <v>160</v>
       </c>
-      <c r="B58" s="16">
+      <c r="B58" s="27">
         <v>0</v>
       </c>
-      <c r="C58" s="13" t="s">
+      <c r="C58" s="24" t="s">
         <v>109</v>
       </c>
     </row>
@@ -3264,10 +3258,10 @@
       <c r="A59" t="s">
         <v>161</v>
       </c>
-      <c r="B59" s="16">
+      <c r="B59" s="27">
         <v>0</v>
       </c>
-      <c r="C59" s="13" t="s">
+      <c r="C59" s="24" t="s">
         <v>111</v>
       </c>
     </row>
@@ -3275,10 +3269,10 @@
       <c r="A60" t="s">
         <v>162</v>
       </c>
-      <c r="B60" s="16">
+      <c r="B60" s="27">
         <v>0</v>
       </c>
-      <c r="C60" s="13" t="s">
+      <c r="C60" s="24" t="s">
         <v>113</v>
       </c>
     </row>
@@ -3286,10 +3280,10 @@
       <c r="A61" t="s">
         <v>163</v>
       </c>
-      <c r="B61" s="9">
+      <c r="B61" s="20">
         <v>1</v>
       </c>
-      <c r="C61" s="22" t="s">
+      <c r="C61" s="33" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3297,10 +3291,10 @@
       <c r="A62" t="s">
         <v>164</v>
       </c>
-      <c r="B62" s="9">
+      <c r="B62" s="20">
         <v>15</v>
       </c>
-      <c r="C62" s="22" t="s">
+      <c r="C62" s="33" t="s">
         <v>105</v>
       </c>
     </row>
@@ -3308,10 +3302,10 @@
       <c r="A63" t="s">
         <v>165</v>
       </c>
-      <c r="B63" s="16">
+      <c r="B63" s="27">
         <v>0</v>
       </c>
-      <c r="C63" s="13" t="s">
+      <c r="C63" s="24" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3319,10 +3313,10 @@
       <c r="A64" t="s">
         <v>166</v>
       </c>
-      <c r="B64" s="16">
+      <c r="B64" s="27">
         <v>1</v>
       </c>
-      <c r="C64" s="13" t="s">
+      <c r="C64" s="24" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3330,10 +3324,10 @@
       <c r="A65" t="s">
         <v>167</v>
       </c>
-      <c r="B65" s="16">
+      <c r="B65" s="27">
         <v>0.5</v>
       </c>
-      <c r="C65" s="13" t="s">
+      <c r="C65" s="24" t="s">
         <v>113</v>
       </c>
     </row>
@@ -3341,10 +3335,10 @@
       <c r="A66" t="s">
         <v>168</v>
       </c>
-      <c r="B66" s="16">
+      <c r="B66" s="27">
         <v>0.2</v>
       </c>
-      <c r="C66" s="13" t="s">
+      <c r="C66" s="24" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3352,10 +3346,10 @@
       <c r="A67" t="s">
         <v>169</v>
       </c>
-      <c r="B67" s="16">
+      <c r="B67" s="27">
         <v>1</v>
       </c>
-      <c r="C67" s="13" t="s">
+      <c r="C67" s="24" t="s">
         <v>170</v>
       </c>
     </row>
@@ -3363,10 +3357,10 @@
       <c r="A68" t="s">
         <v>171</v>
       </c>
-      <c r="B68" s="16">
+      <c r="B68" s="27">
         <v>1</v>
       </c>
-      <c r="C68" s="13" t="s">
+      <c r="C68" s="24" t="s">
         <v>170</v>
       </c>
     </row>
@@ -3374,10 +3368,10 @@
       <c r="A69" t="s">
         <v>172</v>
       </c>
-      <c r="B69" s="16">
+      <c r="B69" s="27">
         <v>250</v>
       </c>
-      <c r="C69" s="13" t="s">
+      <c r="C69" s="24" t="s">
         <v>113</v>
       </c>
     </row>
@@ -3385,10 +3379,10 @@
       <c r="A70" t="s">
         <v>173</v>
       </c>
-      <c r="B70" s="16">
+      <c r="B70" s="27">
         <v>6.75</v>
       </c>
-      <c r="C70" s="13" t="s">
+      <c r="C70" s="24" t="s">
         <v>174</v>
       </c>
     </row>
@@ -3396,10 +3390,10 @@
       <c r="A71" t="s">
         <v>175</v>
       </c>
-      <c r="B71" s="16">
+      <c r="B71" s="27">
         <v>13.5</v>
       </c>
-      <c r="C71" s="13" t="s">
+      <c r="C71" s="24" t="s">
         <v>105</v>
       </c>
     </row>
@@ -3407,10 +3401,10 @@
       <c r="A72" t="s">
         <v>176</v>
       </c>
-      <c r="B72" s="16">
+      <c r="B72" s="27">
         <v>0</v>
       </c>
-      <c r="C72" s="13" t="s">
+      <c r="C72" s="24" t="s">
         <v>105</v>
       </c>
     </row>
@@ -3418,10 +3412,10 @@
       <c r="A73" t="s">
         <v>177</v>
       </c>
-      <c r="B73" s="16">
+      <c r="B73" s="27">
         <v>1</v>
       </c>
-      <c r="C73" s="13" t="s">
+      <c r="C73" s="24" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3429,10 +3423,10 @@
       <c r="A74" t="s">
         <v>178</v>
       </c>
-      <c r="B74" s="26">
+      <c r="B74" s="37">
         <v>0.5</v>
       </c>
-      <c r="C74" s="13" t="s">
+      <c r="C74" s="24" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3440,10 +3434,10 @@
       <c r="A75" t="s">
         <v>179</v>
       </c>
-      <c r="B75" s="16">
+      <c r="B75" s="27">
         <v>0.97</v>
       </c>
-      <c r="C75" s="13" t="s">
+      <c r="C75" s="24" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3451,10 +3445,10 @@
       <c r="A76" t="s">
         <v>180</v>
       </c>
-      <c r="B76" s="16">
+      <c r="B76" s="27">
         <v>0.97</v>
       </c>
-      <c r="C76" s="13" t="s">
+      <c r="C76" s="24" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3462,10 +3456,10 @@
       <c r="A77" t="s">
         <v>181</v>
       </c>
-      <c r="B77" s="16">
+      <c r="B77" s="27">
         <v>0</v>
       </c>
-      <c r="C77" s="13" t="s">
+      <c r="C77" s="24" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3473,10 +3467,10 @@
       <c r="A78" t="s">
         <v>182</v>
       </c>
-      <c r="B78" s="16">
+      <c r="B78" s="27">
         <v>500</v>
       </c>
-      <c r="C78" s="13" t="s">
+      <c r="C78" s="24" t="s">
         <v>109</v>
       </c>
     </row>
@@ -3484,10 +3478,10 @@
       <c r="A79" t="s">
         <v>183</v>
       </c>
-      <c r="B79" s="16">
+      <c r="B79" s="27">
         <v>0</v>
       </c>
-      <c r="C79" s="13" t="s">
+      <c r="C79" s="24" t="s">
         <v>111</v>
       </c>
     </row>
@@ -3495,10 +3489,10 @@
       <c r="A80" t="s">
         <v>184</v>
       </c>
-      <c r="B80" s="16">
+      <c r="B80" s="27">
         <v>13.5</v>
       </c>
-      <c r="C80" s="13" t="s">
+      <c r="C80" s="24" t="s">
         <v>105</v>
       </c>
     </row>
@@ -3506,10 +3500,10 @@
       <c r="A81" t="s">
         <v>185</v>
       </c>
-      <c r="B81" s="16" t="s">
+      <c r="B81" s="27" t="s">
         <v>186</v>
       </c>
-      <c r="C81" s="13" t="s">
+      <c r="C81" s="24" t="s">
         <v>187</v>
       </c>
     </row>
@@ -3517,10 +3511,10 @@
       <c r="A82" t="s">
         <v>188</v>
       </c>
-      <c r="B82" s="16">
+      <c r="B82" s="27">
         <v>1</v>
       </c>
-      <c r="C82" s="13" t="s">
+      <c r="C82" s="24" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3528,10 +3522,10 @@
       <c r="A83" t="s">
         <v>189</v>
       </c>
-      <c r="B83" s="16">
+      <c r="B83" s="27">
         <v>0.2</v>
       </c>
-      <c r="C83" s="13" t="s">
+      <c r="C83" s="24" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3539,10 +3533,10 @@
       <c r="A84" t="s">
         <v>190</v>
       </c>
-      <c r="B84" s="16">
+      <c r="B84" s="27">
         <v>0</v>
       </c>
-      <c r="C84" s="13" t="s">
+      <c r="C84" s="24" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3550,10 +3544,10 @@
       <c r="A85" t="s">
         <v>191</v>
       </c>
-      <c r="B85" s="16">
+      <c r="B85" s="27">
         <v>0.16</v>
       </c>
-      <c r="C85" s="13" t="s">
+      <c r="C85" s="24" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3561,10 +3555,10 @@
       <c r="A86" t="s">
         <v>192</v>
       </c>
-      <c r="B86" s="16">
+      <c r="B86" s="27">
         <v>0</v>
       </c>
-      <c r="C86" s="13" t="s">
+      <c r="C86" s="24" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3572,10 +3566,10 @@
       <c r="A87" t="s">
         <v>193</v>
       </c>
-      <c r="B87" s="16">
+      <c r="B87" s="27">
         <v>0</v>
       </c>
-      <c r="C87" s="13" t="s">
+      <c r="C87" s="24" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3583,10 +3577,10 @@
       <c r="A88" t="s">
         <v>194</v>
       </c>
-      <c r="B88" s="16">
+      <c r="B88" s="27">
         <v>0</v>
       </c>
-      <c r="C88" s="13" t="s">
+      <c r="C88" s="24" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3594,10 +3588,10 @@
       <c r="A89" t="s">
         <v>195</v>
       </c>
-      <c r="B89" s="16">
+      <c r="B89" s="27">
         <v>0.5</v>
       </c>
-      <c r="C89" s="13" t="s">
+      <c r="C89" s="24" t="s">
         <v>107</v>
       </c>
     </row>
@@ -3605,10 +3599,10 @@
       <c r="A90" t="s">
         <v>196</v>
       </c>
-      <c r="B90" s="16">
+      <c r="B90" s="27">
         <v>1100</v>
       </c>
-      <c r="C90" s="13" t="s">
+      <c r="C90" s="24" t="s">
         <v>109</v>
       </c>
     </row>
@@ -3616,10 +3610,10 @@
       <c r="A91" t="s">
         <v>197</v>
       </c>
-      <c r="B91" s="16">
+      <c r="B91" s="27">
         <v>0</v>
       </c>
-      <c r="C91" s="13" t="s">
+      <c r="C91" s="24" t="s">
         <v>111</v>
       </c>
     </row>
@@ -3627,10 +3621,10 @@
       <c r="A92" t="s">
         <v>198</v>
       </c>
-      <c r="B92" s="16">
+      <c r="B92" s="27">
         <v>0</v>
       </c>
-      <c r="C92" s="13" t="s">
+      <c r="C92" s="24" t="s">
         <v>113</v>
       </c>
     </row>
@@ -3638,10 +3632,10 @@
       <c r="A93" t="s">
         <v>199</v>
       </c>
-      <c r="B93" s="16">
+      <c r="B93" s="27">
         <v>20</v>
       </c>
-      <c r="C93" s="13" t="s">
+      <c r="C93" s="24" t="s">
         <v>105</v>
       </c>
     </row>
@@ -3649,10 +3643,10 @@
       <c r="A94" t="s">
         <v>200</v>
       </c>
-      <c r="B94" s="9">
+      <c r="B94" s="20">
         <v>2.68</v>
       </c>
-      <c r="C94" s="22" t="s">
+      <c r="C94" s="33" t="s">
         <v>201</v>
       </c>
     </row>
@@ -3660,10 +3654,10 @@
       <c r="A95" t="s">
         <v>202</v>
       </c>
-      <c r="B95" s="9">
+      <c r="B95" s="20">
         <v>0.9</v>
       </c>
-      <c r="C95" s="22" t="s">
+      <c r="C95" s="33" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3685,153 +3679,153 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.453125" style="18" customWidth="1"/>
-    <col min="2" max="2" width="9.81640625" style="18" customWidth="1"/>
-    <col min="3" max="4" width="6.90625" style="18" customWidth="1"/>
+    <col min="1" max="1" width="12.453125" style="29" customWidth="1"/>
+    <col min="2" max="2" width="9.81640625" style="29" customWidth="1"/>
+    <col min="3" max="4" width="6.90625" style="29" customWidth="1"/>
     <col min="5" max="6" width="8.54296875" customWidth="1"/>
     <col min="7" max="7" width="8.36328125" customWidth="1"/>
     <col min="8" max="1025" width="8.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="21" t="s">
         <v>204</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
     </row>
     <row r="2" spans="1:7" ht="13" x14ac:dyDescent="0.3">
-      <c r="A2" s="10"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
     </row>
     <row r="3" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="38" t="s">
         <v>205</v>
       </c>
-      <c r="B3" s="65" t="s">
+      <c r="B3" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
     </row>
     <row r="4" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="65" t="s">
+      <c r="B4" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
     </row>
     <row r="5" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="B5" s="66" t="s">
+      <c r="B5" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="40" t="s">
         <v>208</v>
       </c>
-      <c r="B6" s="64" t="s">
+      <c r="B6" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="C6" s="64"/>
-      <c r="D6" s="64"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="64"/>
-      <c r="G6" s="64"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
     </row>
     <row r="7" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="40" t="s">
         <v>210</v>
       </c>
-      <c r="B7" s="64" t="s">
+      <c r="B7" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="C7" s="64"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="64"/>
-      <c r="F7" s="64"/>
-      <c r="G7" s="64"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="40" t="s">
         <v>212</v>
       </c>
-      <c r="B8" s="64" t="s">
+      <c r="B8" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="C8" s="64"/>
-      <c r="D8" s="64"/>
-      <c r="E8" s="64"/>
-      <c r="F8" s="64"/>
-      <c r="G8" s="64"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="20" t="s">
         <v>208</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="24" t="s">
         <v>210</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="29" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="B11" s="18">
+      <c r="B11" s="29">
         <v>1000</v>
       </c>
-      <c r="C11" s="18">
-        <v>1000</v>
-      </c>
-      <c r="D11" s="18">
+      <c r="C11" s="29">
+        <v>1200</v>
+      </c>
+      <c r="D11" s="29">
         <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="29" t="s">
         <v>158</v>
       </c>
-      <c r="B12" s="18">
-        <v>20</v>
-      </c>
-      <c r="C12" s="18">
+      <c r="B12" s="29">
+        <v>15</v>
+      </c>
+      <c r="C12" s="29">
         <v>25</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="29">
         <v>5</v>
       </c>
     </row>
@@ -3863,237 +3857,237 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.54296875" style="18" customWidth="1"/>
-    <col min="2" max="2" width="14.453125" style="18" customWidth="1"/>
-    <col min="3" max="3" width="9.1796875" style="18" customWidth="1"/>
-    <col min="4" max="5" width="15" style="18" customWidth="1"/>
-    <col min="6" max="7" width="9.36328125" style="18" customWidth="1"/>
-    <col min="8" max="8" width="8.7265625" style="18" customWidth="1"/>
-    <col min="9" max="9" width="9.36328125" style="18" customWidth="1"/>
-    <col min="10" max="18" width="6.90625" style="18" customWidth="1"/>
-    <col min="19" max="19" width="12.453125" style="18" customWidth="1"/>
-    <col min="20" max="20" width="11.08984375" style="18" customWidth="1"/>
-    <col min="21" max="1023" width="6.90625" style="18" customWidth="1"/>
+    <col min="1" max="1" width="15.54296875" style="29" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" style="29" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" style="29" customWidth="1"/>
+    <col min="4" max="5" width="15" style="29" customWidth="1"/>
+    <col min="6" max="7" width="9.36328125" style="29" customWidth="1"/>
+    <col min="8" max="8" width="8.7265625" style="29" customWidth="1"/>
+    <col min="9" max="9" width="9.36328125" style="29" customWidth="1"/>
+    <col min="10" max="18" width="6.90625" style="29" customWidth="1"/>
+    <col min="19" max="19" width="12.453125" style="29" customWidth="1"/>
+    <col min="20" max="20" width="11.08984375" style="29" customWidth="1"/>
+    <col min="21" max="1023" width="6.90625" style="29" customWidth="1"/>
     <col min="1024" max="1025" width="6.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="21" t="s">
         <v>214</v>
       </c>
-      <c r="I1" s="9"/>
-      <c r="J1" s="13"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I2" s="9"/>
-      <c r="J2" s="13"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="24"/>
     </row>
     <row r="3" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="38" t="s">
         <v>215</v>
       </c>
-      <c r="B3" s="65" t="s">
+      <c r="B3" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="13"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="24"/>
     </row>
     <row r="4" spans="1:12" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="38" t="s">
         <v>217</v>
       </c>
-      <c r="B4" s="65" t="s">
+      <c r="B4" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="13"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="24"/>
     </row>
     <row r="5" spans="1:12" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="38" t="s">
         <v>219</v>
       </c>
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="13"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="24"/>
     </row>
     <row r="6" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="B6" s="64" t="s">
+      <c r="B6" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="C6" s="64"/>
-      <c r="D6" s="64"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="13"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="13"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="24"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="24"/>
     </row>
     <row r="7" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="22" t="s">
         <v>223</v>
       </c>
-      <c r="B7" s="64" t="s">
+      <c r="B7" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="C7" s="64"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="13"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="13"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="24"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="24"/>
     </row>
     <row r="8" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="22" t="s">
         <v>225</v>
       </c>
-      <c r="B8" s="64" t="s">
+      <c r="B8" s="9" t="s">
         <v>226</v>
       </c>
-      <c r="C8" s="64"/>
-      <c r="D8" s="64"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="13"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="13"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="24"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="24"/>
     </row>
     <row r="9" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="22" t="s">
         <v>227</v>
       </c>
-      <c r="B9" s="64" t="s">
+      <c r="B9" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="C9" s="64"/>
-      <c r="D9" s="64"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="13"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="13"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="24"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="24"/>
     </row>
     <row r="10" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="22" t="s">
         <v>229</v>
       </c>
-      <c r="B10" s="64" t="s">
+      <c r="B10" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="C10" s="64"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="13"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="13"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="24"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="24"/>
     </row>
     <row r="11" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="22" t="s">
         <v>231</v>
       </c>
-      <c r="B11" s="64" t="s">
+      <c r="B11" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="C11" s="64"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="13"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="13"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="24"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="24"/>
     </row>
     <row r="12" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="22" t="s">
         <v>233</v>
       </c>
-      <c r="B12" s="64" t="s">
+      <c r="B12" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="C12" s="64"/>
-      <c r="D12" s="64"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="13"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="13"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="24"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="24"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I13" s="9"/>
-      <c r="J13" s="13"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="24"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="29" t="s">
         <v>235</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="29" t="s">
         <v>221</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="29" t="s">
         <v>223</v>
       </c>
-      <c r="D14" s="18" t="s">
+      <c r="D14" s="29" t="s">
         <v>236</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="E14" s="29" t="s">
         <v>237</v>
       </c>
-      <c r="F14" s="18" t="s">
+      <c r="F14" s="29" t="s">
         <v>227</v>
       </c>
-      <c r="G14" s="18" t="s">
+      <c r="G14" s="29" t="s">
         <v>229</v>
       </c>
-      <c r="H14" s="18" t="s">
+      <c r="H14" s="29" t="s">
         <v>231</v>
       </c>
-      <c r="I14" s="18" t="s">
+      <c r="I14" s="29" t="s">
         <v>233</v>
       </c>
-      <c r="L14" s="14"/>
+      <c r="L14" s="25"/>
     </row>
     <row r="15" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="29" t="s">
         <v>238</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="29" t="s">
         <v>239</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="29" t="s">
         <v>186</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="D15" s="29" t="s">
         <v>240</v>
       </c>
-      <c r="E15" s="18" t="s">
+      <c r="E15" s="29" t="s">
         <v>186</v>
       </c>
-      <c r="F15" s="18" t="s">
+      <c r="F15" s="29" t="s">
         <v>241</v>
       </c>
-      <c r="G15" s="18" t="s">
+      <c r="G15" s="29" t="s">
         <v>242</v>
       </c>
-      <c r="H15" s="18" t="s">
+      <c r="H15" s="29" t="s">
         <v>186</v>
       </c>
-      <c r="I15" s="18" t="s">
+      <c r="I15" s="29" t="s">
         <v>243</v>
       </c>
     </row>
@@ -4123,529 +4117,529 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMD38"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.6328125" customWidth="1"/>
-    <col min="2" max="4" width="13.08984375" style="18" customWidth="1"/>
-    <col min="5" max="1018" width="6.90625" style="18" customWidth="1"/>
+    <col min="2" max="4" width="13.08984375" style="29" customWidth="1"/>
+    <col min="5" max="1018" width="6.90625" style="29" customWidth="1"/>
     <col min="1019" max="1025" width="11.54296875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="21" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="30"/>
+      <c r="A2" s="41"/>
     </row>
     <row r="3" spans="1:5" ht="23.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="38" t="s">
         <v>244</v>
       </c>
-      <c r="B3" s="65" t="s">
+      <c r="B3" s="8" t="s">
         <v>245</v>
       </c>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="31"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="42"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="43" t="s">
         <v>246</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="43" t="s">
         <v>247</v>
       </c>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="43" t="s">
         <v>248</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="43" t="s">
         <v>249</v>
       </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="43" t="s">
         <v>250</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="43" t="s">
         <v>251</v>
       </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="43" t="s">
         <v>252</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="43" t="s">
         <v>251</v>
       </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="43" t="s">
         <v>253</v>
       </c>
-      <c r="B8" s="32" t="s">
-        <v>350</v>
-      </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
+      <c r="B8" s="43" t="s">
+        <v>251</v>
+      </c>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="43" t="s">
         <v>254</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="43" t="s">
         <v>251</v>
       </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="43" t="s">
         <v>255</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="43" t="s">
         <v>251</v>
       </c>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="43" t="s">
         <v>256</v>
       </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="43" t="s">
         <v>257</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="43" t="s">
         <v>258</v>
       </c>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="44"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="43" t="s">
         <v>259</v>
       </c>
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="43" t="s">
         <v>260</v>
       </c>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="44"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="43" t="s">
         <v>261</v>
       </c>
-      <c r="B14" s="32" t="s">
+      <c r="B14" s="43" t="s">
         <v>262</v>
       </c>
-      <c r="C14" s="33"/>
-      <c r="D14" s="33"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="43" t="s">
         <v>263</v>
       </c>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="43" t="s">
         <v>264</v>
       </c>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
     </row>
     <row r="17" spans="1:5" ht="123" x14ac:dyDescent="0.25">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="45" t="s">
         <v>246</v>
       </c>
-      <c r="B17" s="35" t="s">
+      <c r="B17" s="46" t="s">
         <v>265</v>
       </c>
-      <c r="C17" s="35" t="s">
+      <c r="C17" s="46" t="s">
         <v>266</v>
       </c>
-      <c r="D17" s="35" t="s">
+      <c r="D17" s="46" t="s">
         <v>267</v>
       </c>
-      <c r="E17" s="35" t="s">
+      <c r="E17" s="46" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="45" t="s">
         <v>269</v>
       </c>
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="36" t="s">
+      <c r="C18" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="36" t="s">
+      <c r="D18" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="E18" s="36" t="s">
+      <c r="E18" s="47" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="34" t="s">
+      <c r="A19" s="45" t="s">
         <v>248</v>
       </c>
-      <c r="B19" s="36" t="s">
+      <c r="B19" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="36" t="s">
+      <c r="C19" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="36" t="s">
+      <c r="D19" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="E19" s="36" t="s">
+      <c r="E19" s="47" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="34" t="s">
+      <c r="A20" s="45" t="s">
         <v>270</v>
       </c>
-      <c r="B20" s="36" t="s">
+      <c r="B20" s="47" t="s">
         <v>186</v>
       </c>
-      <c r="C20" s="36" t="s">
+      <c r="C20" s="47" t="s">
         <v>271</v>
       </c>
-      <c r="D20" s="36" t="s">
+      <c r="D20" s="47" t="s">
         <v>271</v>
       </c>
-      <c r="E20" s="36" t="s">
+      <c r="E20" s="47" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="34" t="s">
+      <c r="A21" s="45" t="s">
         <v>272</v>
       </c>
-      <c r="B21" s="36" t="s">
+      <c r="B21" s="47" t="s">
         <v>186</v>
       </c>
-      <c r="C21" s="36" t="s">
+      <c r="C21" s="47" t="s">
         <v>186</v>
       </c>
-      <c r="D21" s="36" t="s">
+      <c r="D21" s="47" t="s">
         <v>186</v>
       </c>
-      <c r="E21" s="36" t="s">
+      <c r="E21" s="47" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="34" t="s">
+      <c r="A22" s="45" t="s">
         <v>273</v>
       </c>
-      <c r="B22" s="36" t="s">
+      <c r="B22" s="47" t="s">
         <v>186</v>
       </c>
-      <c r="C22" s="36" t="s">
+      <c r="C22" s="47" t="s">
         <v>186</v>
       </c>
-      <c r="D22" s="36" t="s">
+      <c r="D22" s="47" t="s">
         <v>271</v>
       </c>
-      <c r="E22" s="36" t="s">
+      <c r="E22" s="47" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="37" t="s">
+      <c r="A23" s="48" t="s">
         <v>274</v>
       </c>
-      <c r="B23" s="36" t="s">
+      <c r="B23" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="36" t="s">
+      <c r="C23" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="36" t="s">
+      <c r="D23" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="E23" s="36" t="s">
+      <c r="E23" s="47" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="37" t="s">
+      <c r="A24" s="48" t="s">
         <v>275</v>
       </c>
-      <c r="B24" s="36" t="s">
+      <c r="B24" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="C24" s="36" t="s">
+      <c r="C24" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="D24" s="36" t="s">
+      <c r="D24" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="E24" s="36" t="s">
+      <c r="E24" s="47" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="34" t="s">
+      <c r="A25" s="45" t="s">
         <v>276</v>
       </c>
-      <c r="B25" s="36" t="s">
+      <c r="B25" s="47" t="s">
         <v>271</v>
       </c>
-      <c r="C25" s="36" t="s">
+      <c r="C25" s="47" t="s">
         <v>271</v>
       </c>
-      <c r="D25" s="36" t="s">
+      <c r="D25" s="47" t="s">
         <v>271</v>
       </c>
-      <c r="E25" s="36" t="s">
+      <c r="E25" s="47" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="34" t="s">
+      <c r="A26" s="45" t="s">
         <v>277</v>
       </c>
-      <c r="B26" s="36" t="s">
+      <c r="B26" s="47" t="s">
         <v>271</v>
       </c>
-      <c r="C26" s="36" t="s">
+      <c r="C26" s="47" t="s">
         <v>271</v>
       </c>
-      <c r="D26" s="36" t="s">
+      <c r="D26" s="47" t="s">
         <v>271</v>
       </c>
-      <c r="E26" s="36" t="s">
+      <c r="E26" s="47" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="48" t="s">
         <v>278</v>
       </c>
-      <c r="B27" s="36" t="s">
+      <c r="B27" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="36" t="s">
+      <c r="C27" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="D27" s="36" t="s">
+      <c r="D27" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="E27" s="36" t="s">
+      <c r="E27" s="47" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="34" t="s">
+      <c r="A28" s="45" t="s">
         <v>279</v>
       </c>
-      <c r="B28" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="C28" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="D28" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="E28" s="36" t="s">
-        <v>349</v>
+      <c r="B28" s="47" t="s">
+        <v>271</v>
+      </c>
+      <c r="C28" s="47" t="s">
+        <v>271</v>
+      </c>
+      <c r="D28" s="47" t="s">
+        <v>271</v>
+      </c>
+      <c r="E28" s="47" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="37" t="s">
+      <c r="A29" s="48" t="s">
         <v>280</v>
       </c>
-      <c r="B29" s="36" t="s">
+      <c r="B29" s="47" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="47" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" s="47" t="s">
+        <v>39</v>
+      </c>
+      <c r="E29" s="47" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="48" t="s">
+        <v>281</v>
+      </c>
+      <c r="B30" s="47" t="s">
+        <v>282</v>
+      </c>
+      <c r="C30" s="47" t="s">
+        <v>282</v>
+      </c>
+      <c r="D30" s="47" t="s">
+        <v>282</v>
+      </c>
+      <c r="E30" s="47" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="45" t="s">
+        <v>283</v>
+      </c>
+      <c r="B31" s="47" t="s">
+        <v>186</v>
+      </c>
+      <c r="C31" s="47" t="s">
+        <v>186</v>
+      </c>
+      <c r="D31" s="47" t="s">
+        <v>186</v>
+      </c>
+      <c r="E31" s="47" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="45" t="s">
+        <v>284</v>
+      </c>
+      <c r="B32" s="47" t="s">
+        <v>186</v>
+      </c>
+      <c r="C32" s="47" t="s">
+        <v>186</v>
+      </c>
+      <c r="D32" s="47" t="s">
+        <v>186</v>
+      </c>
+      <c r="E32" s="47" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="36" t="s">
+      <c r="C33" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="D29" s="36" t="s">
+      <c r="D33" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="E29" s="36" t="s">
+      <c r="E33" s="47" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="37" t="s">
-        <v>281</v>
-      </c>
-      <c r="B30" s="36" t="s">
-        <v>282</v>
-      </c>
-      <c r="C30" s="36" t="s">
-        <v>282</v>
-      </c>
-      <c r="D30" s="36" t="s">
-        <v>282</v>
-      </c>
-      <c r="E30" s="36" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="34" t="s">
-        <v>283</v>
-      </c>
-      <c r="B31" s="36" t="s">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="45" t="s">
+        <v>257</v>
+      </c>
+      <c r="B34" s="47" t="s">
+        <v>285</v>
+      </c>
+      <c r="C34" s="47" t="s">
+        <v>285</v>
+      </c>
+      <c r="D34" s="47" t="s">
+        <v>285</v>
+      </c>
+      <c r="E34" s="47" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="45" t="s">
+        <v>259</v>
+      </c>
+      <c r="B35" s="47" t="s">
+        <v>286</v>
+      </c>
+      <c r="C35" s="47" t="s">
+        <v>286</v>
+      </c>
+      <c r="D35" s="47" t="s">
+        <v>286</v>
+      </c>
+      <c r="E35" s="47" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="45" t="s">
+        <v>261</v>
+      </c>
+      <c r="B36" s="47" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" s="47" t="s">
+        <v>39</v>
+      </c>
+      <c r="D36" s="47" t="s">
+        <v>39</v>
+      </c>
+      <c r="E36" s="47" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="45" t="s">
+        <v>263</v>
+      </c>
+      <c r="B37" s="47" t="s">
         <v>186</v>
       </c>
-      <c r="C31" s="36" t="s">
+      <c r="C37" s="47" t="s">
         <v>186</v>
       </c>
-      <c r="D31" s="36" t="s">
+      <c r="D37" s="47" t="s">
         <v>186</v>
       </c>
-      <c r="E31" s="36" t="s">
+      <c r="E37" s="47" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="34" t="s">
-        <v>284</v>
-      </c>
-      <c r="B32" s="36" t="s">
-        <v>186</v>
-      </c>
-      <c r="C32" s="36" t="s">
-        <v>186</v>
-      </c>
-      <c r="D32" s="36" t="s">
-        <v>186</v>
-      </c>
-      <c r="E32" s="36" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="B33" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="C33" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="D33" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="E33" s="36" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="34" t="s">
-        <v>257</v>
-      </c>
-      <c r="B34" s="36" t="s">
-        <v>285</v>
-      </c>
-      <c r="C34" s="36" t="s">
-        <v>285</v>
-      </c>
-      <c r="D34" s="36" t="s">
-        <v>285</v>
-      </c>
-      <c r="E34" s="36" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="34" t="s">
-        <v>259</v>
-      </c>
-      <c r="B35" s="36" t="s">
-        <v>286</v>
-      </c>
-      <c r="C35" s="36" t="s">
-        <v>286</v>
-      </c>
-      <c r="D35" s="36" t="s">
-        <v>286</v>
-      </c>
-      <c r="E35" s="36" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="34" t="s">
-        <v>261</v>
-      </c>
-      <c r="B36" s="36" t="s">
-        <v>39</v>
-      </c>
-      <c r="C36" s="36" t="s">
-        <v>39</v>
-      </c>
-      <c r="D36" s="36" t="s">
-        <v>39</v>
-      </c>
-      <c r="E36" s="36" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="34" t="s">
-        <v>263</v>
-      </c>
-      <c r="B37" s="36" t="s">
-        <v>186</v>
-      </c>
-      <c r="C37" s="36" t="s">
-        <v>186</v>
-      </c>
-      <c r="D37" s="36" t="s">
-        <v>186</v>
-      </c>
-      <c r="E37" s="36" t="s">
-        <v>186</v>
-      </c>
-      <c r="F37" s="36"/>
+      <c r="F37" s="47"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="34" t="s">
+      <c r="A38" s="45" t="s">
         <v>287</v>
       </c>
-      <c r="B38" s="38" t="s">
+      <c r="B38" s="49" t="s">
         <v>288</v>
       </c>
-      <c r="C38" s="38" t="s">
+      <c r="C38" s="49" t="s">
         <v>288</v>
       </c>
-      <c r="D38" s="38" t="s">
+      <c r="D38" s="49" t="s">
         <v>288</v>
       </c>
-      <c r="E38" s="38" t="s">
+      <c r="E38" s="49" t="s">
         <v>288</v>
       </c>
     </row>
@@ -4684,509 +4678,509 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="50" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="39"/>
+      <c r="A2" s="50"/>
     </row>
     <row r="3" spans="1:8" ht="23.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="38" t="s">
         <v>290</v>
       </c>
-      <c r="B3" s="65" t="s">
+      <c r="B3" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="43" t="s">
         <v>292</v>
       </c>
-      <c r="B4" s="67" t="s">
+      <c r="B4" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="67"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="43" t="s">
         <v>294</v>
       </c>
-      <c r="B5" s="67" t="s">
+      <c r="B5" s="6" t="s">
         <v>295</v>
       </c>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="67"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
     </row>
     <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="51" t="s">
         <v>296</v>
       </c>
-      <c r="B6" s="65" t="s">
+      <c r="B6" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="65"/>
-      <c r="G6" s="65"/>
-      <c r="H6" s="65"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
     </row>
     <row r="7" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="51" t="s">
         <v>298</v>
       </c>
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="8" t="s">
         <v>299</v>
       </c>
-      <c r="C7" s="65"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="65"/>
-      <c r="F7" s="65"/>
-      <c r="G7" s="65"/>
-      <c r="H7" s="65"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
     </row>
     <row r="8" spans="1:8" ht="41" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="51" t="s">
         <v>300</v>
       </c>
-      <c r="B8" s="65" t="s">
+      <c r="B8" s="8" t="s">
         <v>301</v>
       </c>
-      <c r="C8" s="65"/>
-      <c r="D8" s="65"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="65"/>
-      <c r="G8" s="65"/>
-      <c r="H8" s="65"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="41" t="s">
+      <c r="A10" s="52" t="s">
         <v>302</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="53" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="43" t="s">
+      <c r="A11" s="54" t="s">
         <v>304</v>
       </c>
-      <c r="B11" s="43">
+      <c r="B11" s="54">
         <v>0.28622953868737899</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="54" t="s">
         <v>305</v>
       </c>
-      <c r="B12" s="43">
+      <c r="B12" s="54">
         <v>0.25807310904584102</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="54" t="s">
         <v>306</v>
       </c>
-      <c r="B13" s="43">
+      <c r="B13" s="54">
         <v>0.23396226376115001</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="43" t="s">
+      <c r="A14" s="54" t="s">
         <v>307</v>
       </c>
-      <c r="B14" s="43">
+      <c r="B14" s="54">
         <v>0.22173508850563001</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E16" s="70" t="s">
+      <c r="E16" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="F16" s="70"/>
-      <c r="G16" s="70"/>
-      <c r="H16" s="70"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="45" t="s">
+      <c r="A17" s="56" t="s">
         <v>302</v>
       </c>
-      <c r="B17" s="45" t="s">
+      <c r="B17" s="56" t="s">
         <v>309</v>
       </c>
-      <c r="C17" s="46" t="s">
+      <c r="C17" s="57" t="s">
         <v>294</v>
       </c>
-      <c r="D17" s="47" t="s">
+      <c r="D17" s="58" t="s">
         <v>303</v>
       </c>
-      <c r="E17" s="44" t="s">
+      <c r="E17" s="55" t="s">
         <v>310</v>
       </c>
-      <c r="F17" s="44" t="s">
+      <c r="F17" s="55" t="s">
         <v>311</v>
       </c>
-      <c r="G17" s="44" t="s">
+      <c r="G17" s="55" t="s">
         <v>312</v>
       </c>
-      <c r="H17" s="44" t="s">
+      <c r="H17" s="55" t="s">
         <v>313</v>
       </c>
-      <c r="I17" s="44" t="s">
+      <c r="I17" s="55" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="71" t="s">
+      <c r="A18" s="4" t="s">
         <v>315</v>
       </c>
-      <c r="B18" s="48" t="s">
+      <c r="B18" s="59" t="s">
         <v>316</v>
       </c>
-      <c r="C18" s="49" t="s">
+      <c r="C18" s="60" t="s">
         <v>317</v>
       </c>
-      <c r="D18" s="50">
+      <c r="D18" s="61">
         <v>0.51388888888888895</v>
       </c>
-      <c r="E18" s="51"/>
-      <c r="F18" s="44"/>
-      <c r="G18" s="44"/>
-      <c r="H18" s="44"/>
-      <c r="I18" s="52" t="s">
+      <c r="E18" s="62"/>
+      <c r="F18" s="55"/>
+      <c r="G18" s="55"/>
+      <c r="H18" s="55"/>
+      <c r="I18" s="63" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="71"/>
-      <c r="B19" s="53" t="s">
+      <c r="A19" s="4"/>
+      <c r="B19" s="64" t="s">
         <v>319</v>
       </c>
-      <c r="C19" s="54" t="s">
+      <c r="C19" s="65" t="s">
         <v>320</v>
       </c>
-      <c r="D19" s="55">
+      <c r="D19" s="66">
         <v>0.48611111111111099</v>
       </c>
-      <c r="E19" s="51"/>
-      <c r="F19" s="44"/>
-      <c r="G19" s="44"/>
-      <c r="H19" s="44"/>
-      <c r="I19" s="52" t="s">
+      <c r="E19" s="62"/>
+      <c r="F19" s="55"/>
+      <c r="G19" s="55"/>
+      <c r="H19" s="55"/>
+      <c r="I19" s="63" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="71" t="s">
+      <c r="A20" s="4" t="s">
         <v>321</v>
       </c>
-      <c r="B20" s="48" t="s">
+      <c r="B20" s="59" t="s">
         <v>322</v>
       </c>
-      <c r="C20" s="49" t="s">
+      <c r="C20" s="60" t="s">
         <v>323</v>
       </c>
-      <c r="D20" s="50">
+      <c r="D20" s="61">
         <v>0.25987103174603199</v>
       </c>
-      <c r="E20" s="51"/>
-      <c r="F20" s="44"/>
-      <c r="G20" s="44"/>
-      <c r="H20" s="44"/>
-      <c r="I20" s="52" t="s">
+      <c r="E20" s="62"/>
+      <c r="F20" s="55"/>
+      <c r="G20" s="55"/>
+      <c r="H20" s="55"/>
+      <c r="I20" s="63" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="71"/>
-      <c r="B21" s="56" t="s">
+      <c r="A21" s="4"/>
+      <c r="B21" s="67" t="s">
         <v>324</v>
       </c>
-      <c r="C21" s="43" t="s">
+      <c r="C21" s="54" t="s">
         <v>325</v>
       </c>
-      <c r="D21" s="57">
+      <c r="D21" s="68">
         <v>0.23849206349206301</v>
       </c>
-      <c r="E21" s="51"/>
-      <c r="F21" s="44"/>
-      <c r="G21" s="44"/>
-      <c r="H21" s="44"/>
-      <c r="I21" s="52" t="s">
+      <c r="E21" s="62"/>
+      <c r="F21" s="55"/>
+      <c r="G21" s="55"/>
+      <c r="H21" s="55"/>
+      <c r="I21" s="63" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="71"/>
-      <c r="B22" s="56" t="s">
+      <c r="A22" s="4"/>
+      <c r="B22" s="67" t="s">
         <v>326</v>
       </c>
-      <c r="C22" s="43" t="s">
+      <c r="C22" s="54" t="s">
         <v>327</v>
       </c>
-      <c r="D22" s="57">
+      <c r="D22" s="68">
         <v>0.246825396825397</v>
       </c>
-      <c r="E22" s="58">
+      <c r="E22" s="69">
         <v>2.75</v>
       </c>
-      <c r="F22" s="52" t="s">
+      <c r="F22" s="63" t="s">
         <v>186</v>
       </c>
-      <c r="G22" s="52">
+      <c r="G22" s="63">
         <v>1.88</v>
       </c>
-      <c r="H22" s="52">
+      <c r="H22" s="63">
         <v>3</v>
       </c>
-      <c r="I22" s="52" t="s">
+      <c r="I22" s="63" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="71"/>
-      <c r="B23" s="53" t="s">
+      <c r="A23" s="4"/>
+      <c r="B23" s="64" t="s">
         <v>328</v>
       </c>
-      <c r="C23" s="54" t="s">
+      <c r="C23" s="65" t="s">
         <v>329</v>
       </c>
-      <c r="D23" s="55">
+      <c r="D23" s="66">
         <v>0.25481150793650797</v>
       </c>
-      <c r="E23" s="58">
+      <c r="E23" s="69">
         <v>2.25</v>
       </c>
-      <c r="F23" s="52" t="s">
+      <c r="F23" s="63" t="s">
         <v>186</v>
       </c>
-      <c r="G23" s="52">
+      <c r="G23" s="63">
         <v>1.5</v>
       </c>
-      <c r="H23" s="52">
+      <c r="H23" s="63">
         <v>3</v>
       </c>
-      <c r="I23" s="52" t="s">
+      <c r="I23" s="63" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="72" t="s">
+      <c r="A24" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="B24" s="59" t="s">
+      <c r="B24" s="70" t="s">
         <v>331</v>
       </c>
-      <c r="C24" s="43" t="s">
+      <c r="C24" s="54" t="s">
         <v>332</v>
       </c>
-      <c r="D24" s="57">
+      <c r="D24" s="68">
         <v>0.26535443722943702</v>
       </c>
-      <c r="E24" s="58">
+      <c r="E24" s="69">
         <v>2</v>
       </c>
-      <c r="F24" s="52" t="s">
+      <c r="F24" s="63" t="s">
         <v>186</v>
       </c>
-      <c r="G24" s="52">
+      <c r="G24" s="63">
         <v>2.6</v>
       </c>
-      <c r="H24" s="52">
+      <c r="H24" s="63">
         <v>2.17</v>
       </c>
-      <c r="I24" s="52" t="s">
+      <c r="I24" s="63" t="s">
         <v>333</v>
       </c>
-      <c r="N24" s="68"/>
+      <c r="N24" s="2"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="72"/>
-      <c r="B25" s="59" t="s">
+      <c r="A25" s="3"/>
+      <c r="B25" s="70" t="s">
         <v>334</v>
       </c>
-      <c r="C25" s="43" t="s">
+      <c r="C25" s="54" t="s">
         <v>335</v>
       </c>
-      <c r="D25" s="57">
+      <c r="D25" s="68">
         <v>0.39644209956710003</v>
       </c>
-      <c r="E25" s="51"/>
-      <c r="F25" s="44"/>
-      <c r="G25" s="44"/>
-      <c r="H25" s="44"/>
-      <c r="I25" s="52" t="s">
+      <c r="E25" s="62"/>
+      <c r="F25" s="55"/>
+      <c r="G25" s="55"/>
+      <c r="H25" s="55"/>
+      <c r="I25" s="63" t="s">
         <v>318</v>
       </c>
-      <c r="N25" s="68"/>
+      <c r="N25" s="2"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="72"/>
-      <c r="B26" s="60" t="s">
+      <c r="A26" s="3"/>
+      <c r="B26" s="71" t="s">
         <v>336</v>
       </c>
-      <c r="C26" s="54" t="s">
+      <c r="C26" s="65" t="s">
         <v>337</v>
       </c>
-      <c r="D26" s="55">
+      <c r="D26" s="66">
         <v>0.33820346320346301</v>
       </c>
-      <c r="E26" s="58">
+      <c r="E26" s="69">
         <v>2.57</v>
       </c>
-      <c r="F26" s="52" t="s">
+      <c r="F26" s="63" t="s">
         <v>186</v>
       </c>
-      <c r="G26" s="52">
+      <c r="G26" s="63">
         <v>1.71</v>
       </c>
-      <c r="H26" s="52">
+      <c r="H26" s="63">
         <v>2.14</v>
       </c>
-      <c r="I26" s="52" t="s">
+      <c r="I26" s="63" t="s">
         <v>333</v>
       </c>
-      <c r="N26" s="68"/>
+      <c r="N26" s="2"/>
     </row>
     <row r="27" spans="1:14" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="69" t="s">
+      <c r="A27" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="B27" s="61" t="s">
+      <c r="B27" s="72" t="s">
         <v>339</v>
       </c>
-      <c r="C27" s="49" t="s">
+      <c r="C27" s="60" t="s">
         <v>340</v>
       </c>
-      <c r="D27" s="50">
+      <c r="D27" s="61">
         <v>0.25580808080808098</v>
       </c>
-      <c r="E27" s="58">
+      <c r="E27" s="69">
         <v>0</v>
       </c>
-      <c r="F27" s="52" t="s">
+      <c r="F27" s="63" t="s">
         <v>186</v>
       </c>
-      <c r="G27" s="52">
+      <c r="G27" s="63">
         <v>0.77</v>
       </c>
-      <c r="H27" s="52">
+      <c r="H27" s="63">
         <v>0.44</v>
       </c>
-      <c r="I27" s="52" t="s">
+      <c r="I27" s="63" t="s">
         <v>318</v>
       </c>
-      <c r="J27" s="14" t="s">
+      <c r="J27" s="25" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="69"/>
-      <c r="B28" s="59" t="s">
+      <c r="A28" s="1"/>
+      <c r="B28" s="70" t="s">
         <v>342</v>
       </c>
-      <c r="C28" s="43" t="s">
+      <c r="C28" s="54" t="s">
         <v>343</v>
       </c>
-      <c r="D28" s="57">
+      <c r="D28" s="68">
         <v>0.38377525252525302</v>
       </c>
-      <c r="E28" s="58">
+      <c r="E28" s="69">
         <v>2.63</v>
       </c>
-      <c r="F28" s="52" t="s">
+      <c r="F28" s="63" t="s">
         <v>186</v>
       </c>
-      <c r="G28" s="52">
+      <c r="G28" s="63">
         <v>1</v>
       </c>
-      <c r="H28" s="52">
+      <c r="H28" s="63">
         <v>1.88</v>
       </c>
-      <c r="I28" s="52" t="s">
+      <c r="I28" s="63" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="69"/>
-      <c r="B29" s="60" t="s">
+      <c r="A29" s="1"/>
+      <c r="B29" s="71" t="s">
         <v>344</v>
       </c>
-      <c r="C29" s="54" t="s">
+      <c r="C29" s="65" t="s">
         <v>345</v>
       </c>
-      <c r="D29" s="55">
+      <c r="D29" s="66">
         <v>0.360416666666667</v>
       </c>
-      <c r="E29" s="58">
+      <c r="E29" s="69">
         <v>1.63</v>
       </c>
-      <c r="F29" s="52" t="s">
+      <c r="F29" s="63" t="s">
         <v>186</v>
       </c>
-      <c r="G29" s="52">
+      <c r="G29" s="63">
         <v>1.5</v>
       </c>
-      <c r="H29" s="52">
+      <c r="H29" s="63">
         <v>2.63</v>
       </c>
-      <c r="I29" s="52" t="s">
+      <c r="I29" s="63" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="70" t="s">
+      <c r="A32" s="5" t="s">
         <v>300</v>
       </c>
-      <c r="B32" s="70"/>
+      <c r="B32" s="5"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="44" t="s">
+      <c r="A33" s="55" t="s">
         <v>346</v>
       </c>
-      <c r="B33" s="44" t="s">
+      <c r="B33" s="55" t="s">
         <v>347</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="43" t="str">
+      <c r="A34" s="54" t="str">
         <f>IF(input_sensitivity!A11 = "","",input_sensitivity!A11)</f>
         <v>pv_cost_investment</v>
       </c>
-      <c r="B34" s="43" t="b">
+      <c r="B34" s="54" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="43" t="str">
+      <c r="A35" s="54" t="str">
         <f>IF(input_sensitivity!A12 = "","",input_sensitivity!A12)</f>
         <v>pv_lifetime</v>
       </c>
-      <c r="B35" s="43" t="b">
+      <c r="B35" s="54" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Decrease number of simulations in xslx
</commit_message>
<xml_diff>
--- a/inputs/test_input_template.xlsx
+++ b/inputs/test_input_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -1414,39 +1414,6 @@
   </cellStyleXfs>
   <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1603,6 +1570,39 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1969,179 +1969,179 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
     </row>
     <row r="3" spans="2:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B3" s="12"/>
-      <c r="C3" s="13" t="s">
+      <c r="B3" s="1"/>
+      <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
     </row>
     <row r="4" spans="2:6" ht="13" x14ac:dyDescent="0.3">
-      <c r="B4" s="12"/>
-      <c r="C4" s="14" t="s">
+      <c r="B4" s="1"/>
+      <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="12"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
     </row>
     <row r="6" spans="2:6" ht="23.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="12"/>
-      <c r="C6" s="11" t="s">
+      <c r="B6" s="1"/>
+      <c r="C6" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="12"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="1"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="12"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="12" t="s">
+      <c r="B7" s="1"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="12"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="12" t="s">
+      <c r="B8" s="1"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="12"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="12" t="s">
+      <c r="B9" s="1"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="12"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="12" t="s">
+      <c r="B10" s="1"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="12"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="12" t="s">
+      <c r="B11" s="1"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="12"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="12" t="s">
+      <c r="B12" s="1"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="12"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
     </row>
     <row r="14" spans="2:6" ht="13" x14ac:dyDescent="0.3">
-      <c r="B14" s="12"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="16" t="s">
+      <c r="B14" s="1"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="12"/>
+      <c r="F14" s="1"/>
     </row>
     <row r="15" spans="2:6" ht="13" x14ac:dyDescent="0.25">
-      <c r="B15" s="12"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="17" t="s">
+      <c r="B15" s="1"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="18" t="s">
+      <c r="E15" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="12"/>
+      <c r="F15" s="1"/>
     </row>
     <row r="16" spans="2:6" ht="25" x14ac:dyDescent="0.25">
-      <c r="B16" s="12"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="17" t="s">
+      <c r="B16" s="1"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="19" t="s">
+      <c r="E16" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F16" s="12"/>
+      <c r="F16" s="1"/>
     </row>
     <row r="17" spans="2:6" ht="13" x14ac:dyDescent="0.25">
-      <c r="B17" s="12"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="17" t="s">
+      <c r="B17" s="1"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="18" t="s">
+      <c r="E17" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F17" s="12"/>
+      <c r="F17" s="1"/>
     </row>
     <row r="18" spans="2:6" ht="13" x14ac:dyDescent="0.25">
-      <c r="B18" s="12"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="17" t="s">
+      <c r="B18" s="1"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="18" t="s">
+      <c r="E18" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F18" s="12"/>
+      <c r="F18" s="1"/>
     </row>
     <row r="19" spans="2:6" ht="13" x14ac:dyDescent="0.25">
-      <c r="B19" s="12"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="17" t="s">
+      <c r="B19" s="1"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="18" t="s">
+      <c r="E19" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F19" s="12"/>
+      <c r="F19" s="1"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="12"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
@@ -2161,121 +2161,121 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.08984375" customWidth="1"/>
     <col min="2" max="2" width="33.36328125" customWidth="1"/>
-    <col min="3" max="3" width="18.6328125" style="20" customWidth="1"/>
+    <col min="3" max="3" width="18.6328125" style="9" customWidth="1"/>
     <col min="4" max="1025" width="8.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="13" x14ac:dyDescent="0.25">
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
     </row>
     <row r="4" spans="1:6" ht="13" x14ac:dyDescent="0.25">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
     </row>
     <row r="5" spans="1:6" ht="13" x14ac:dyDescent="0.3">
-      <c r="A5" s="21"/>
-      <c r="B5" s="22" t="s">
+      <c r="A5" s="10"/>
+      <c r="B5" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
     </row>
     <row r="6" spans="1:6" ht="13" x14ac:dyDescent="0.3">
-      <c r="A6" s="21"/>
-      <c r="B6" s="22" t="s">
+      <c r="A6" s="10"/>
+      <c r="B6" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
     </row>
     <row r="7" spans="1:6" ht="13" x14ac:dyDescent="0.3">
-      <c r="A7" s="21"/>
-      <c r="B7" s="22" t="s">
+      <c r="A7" s="10"/>
+      <c r="B7" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="63" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
+      <c r="D7" s="63"/>
+      <c r="E7" s="63"/>
+      <c r="F7" s="63"/>
     </row>
     <row r="8" spans="1:6" ht="13" x14ac:dyDescent="0.3">
-      <c r="A8" s="21"/>
-      <c r="B8" s="22" t="s">
+      <c r="A8" s="10"/>
+      <c r="B8" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="63" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
+      <c r="D8" s="63"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="63"/>
     </row>
     <row r="9" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="21"/>
-      <c r="B9" s="22" t="s">
+      <c r="A9" s="10"/>
+      <c r="B9" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
     </row>
     <row r="10" spans="1:6" ht="13" x14ac:dyDescent="0.3">
-      <c r="A10" s="21"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="24"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="13"/>
     </row>
     <row r="11" spans="1:6" ht="13" x14ac:dyDescent="0.3">
-      <c r="A11" s="21"/>
-      <c r="B11" s="25" t="s">
+      <c r="A11" s="10"/>
+      <c r="B11" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="13" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="13" x14ac:dyDescent="0.3">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="10" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2283,7 +2283,7 @@
       <c r="B13" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="15" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2291,15 +2291,15 @@
       <c r="B14" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="26" t="s">
-        <v>41</v>
+      <c r="C14" s="15" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="26" t="s">
+      <c r="C15" s="15" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2307,7 +2307,7 @@
       <c r="B16" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="26" t="s">
+      <c r="C16" s="15" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2315,7 +2315,7 @@
       <c r="B17" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="27">
+      <c r="C17" s="16">
         <v>7</v>
       </c>
     </row>
@@ -2323,7 +2323,7 @@
       <c r="B18" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="28">
+      <c r="C18" s="17">
         <v>43101</v>
       </c>
     </row>
@@ -2331,7 +2331,7 @@
       <c r="B19" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="9" t="s">
         <v>47</v>
       </c>
       <c r="D19" t="s">
@@ -2342,7 +2342,7 @@
       <c r="B20" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="26" t="s">
+      <c r="C20" s="15" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2350,24 +2350,24 @@
       <c r="B21" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="26" t="s">
+      <c r="C21" s="15" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C22" s="29"/>
+      <c r="C22" s="18"/>
     </row>
     <row r="23" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A23" s="21" t="s">
+      <c r="A23" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="29"/>
+      <c r="C23" s="18"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="27" t="s">
+      <c r="C24" s="16" t="s">
         <v>52</v>
       </c>
     </row>
@@ -2375,7 +2375,7 @@
       <c r="B25" t="s">
         <v>53</v>
       </c>
-      <c r="C25" s="26" t="s">
+      <c r="C25" s="15" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2383,7 +2383,7 @@
       <c r="B26" t="s">
         <v>54</v>
       </c>
-      <c r="C26" s="27" t="s">
+      <c r="C26" s="16" t="s">
         <v>55</v>
       </c>
       <c r="D26" t="s">
@@ -2394,25 +2394,25 @@
       <c r="B27" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="27">
+      <c r="C27" s="16">
         <v>0.03</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C28" s="29"/>
+      <c r="C28" s="18"/>
     </row>
     <row r="29" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="21" t="s">
+      <c r="A29" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="30"/>
+      <c r="C29" s="19"/>
     </row>
     <row r="30" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="21"/>
+      <c r="A30" s="10"/>
       <c r="B30" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="31" t="s">
+      <c r="C30" s="20" t="s">
         <v>59</v>
       </c>
       <c r="D30" t="s">
@@ -2420,39 +2420,39 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A31" s="21"/>
+      <c r="A31" s="10"/>
       <c r="B31" t="s">
         <v>61</v>
       </c>
-      <c r="C31" s="20" t="s">
+      <c r="C31" s="9" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A32" s="21"/>
+      <c r="A32" s="10"/>
       <c r="B32" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="27" t="s">
+      <c r="C32" s="16" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C33" s="30"/>
+      <c r="C33" s="19"/>
     </row>
     <row r="34" spans="1:7" ht="13" x14ac:dyDescent="0.3">
-      <c r="A34" s="21" t="s">
+      <c r="A34" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="C34" s="29"/>
-      <c r="D34" s="32"/>
-      <c r="G34" s="32"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="21"/>
+      <c r="G34" s="21"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>65</v>
       </c>
-      <c r="C35" s="26" t="s">
+      <c r="C35" s="15" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2460,7 +2460,7 @@
       <c r="B36" t="s">
         <v>66</v>
       </c>
-      <c r="C36" s="26" t="s">
+      <c r="C36" s="15" t="s">
         <v>39</v>
       </c>
       <c r="D36" t="s">
@@ -2471,7 +2471,7 @@
       <c r="B37" t="s">
         <v>68</v>
       </c>
-      <c r="C37" s="26" t="s">
+      <c r="C37" s="15" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2479,7 +2479,7 @@
       <c r="B38" t="s">
         <v>69</v>
       </c>
-      <c r="C38" s="26" t="s">
+      <c r="C38" s="15" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2487,7 +2487,7 @@
       <c r="B39" t="s">
         <v>70</v>
       </c>
-      <c r="C39" s="26" t="s">
+      <c r="C39" s="15" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2495,7 +2495,7 @@
       <c r="B40" t="s">
         <v>71</v>
       </c>
-      <c r="C40" s="26" t="s">
+      <c r="C40" s="15" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2503,25 +2503,25 @@
       <c r="B41" t="s">
         <v>72</v>
       </c>
-      <c r="C41" s="26" t="s">
+      <c r="C41" s="15" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C42" s="30"/>
+      <c r="C42" s="19"/>
     </row>
     <row r="43" spans="1:7" ht="13" x14ac:dyDescent="0.3">
-      <c r="A43" s="21" t="s">
+      <c r="A43" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B43" s="21"/>
-      <c r="C43" s="30"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="19"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>73</v>
       </c>
-      <c r="C44" s="26" t="s">
+      <c r="C44" s="15" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2529,7 +2529,7 @@
       <c r="B45" t="s">
         <v>74</v>
       </c>
-      <c r="C45" s="26" t="s">
+      <c r="C45" s="15" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2537,24 +2537,24 @@
       <c r="B46" t="s">
         <v>75</v>
       </c>
-      <c r="C46" s="26" t="s">
+      <c r="C46" s="15" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C47" s="30"/>
+      <c r="C47" s="19"/>
     </row>
     <row r="48" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="21" t="s">
+      <c r="A48" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C48" s="29"/>
+      <c r="C48" s="18"/>
     </row>
     <row r="49" spans="2:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>76</v>
       </c>
-      <c r="C49" s="26" t="s">
+      <c r="C49" s="15" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2562,7 +2562,7 @@
       <c r="B50" t="s">
         <v>77</v>
       </c>
-      <c r="C50" s="26" t="s">
+      <c r="C50" s="15" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2570,7 +2570,7 @@
       <c r="B51" t="s">
         <v>78</v>
       </c>
-      <c r="C51" s="26" t="s">
+      <c r="C51" s="15" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2578,7 +2578,7 @@
       <c r="B52" t="s">
         <v>79</v>
       </c>
-      <c r="C52" s="26" t="s">
+      <c r="C52" s="15" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2612,67 +2612,67 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.81640625" customWidth="1"/>
-    <col min="2" max="2" width="6.08984375" style="20" customWidth="1"/>
-    <col min="3" max="3" width="6.6328125" style="33" customWidth="1"/>
+    <col min="2" max="2" width="6.08984375" style="9" customWidth="1"/>
+    <col min="3" max="3" width="6.6328125" style="22" customWidth="1"/>
     <col min="4" max="1023" width="8.6328125" customWidth="1"/>
     <col min="1024" max="1025" width="6.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
     </row>
     <row r="2" spans="1:7" ht="13" x14ac:dyDescent="0.3">
-      <c r="A2" s="21"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
     </row>
     <row r="3" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="64" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
     </row>
     <row r="4" spans="1:7" ht="46.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="64" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
     </row>
     <row r="5" spans="1:7" ht="13" x14ac:dyDescent="0.3">
-      <c r="A5" s="21"/>
-      <c r="B5" s="35"/>
-      <c r="C5" s="36"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="25"/>
     </row>
     <row r="6" spans="1:7" ht="13" x14ac:dyDescent="0.3">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="25" t="s">
         <v>87</v>
       </c>
     </row>
@@ -2680,10 +2680,10 @@
       <c r="A7" t="s">
         <v>88</v>
       </c>
-      <c r="B7" s="27">
+      <c r="B7" s="16">
         <v>0</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="13" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2691,10 +2691,10 @@
       <c r="A8" t="s">
         <v>90</v>
       </c>
-      <c r="B8" s="27">
+      <c r="B8" s="16">
         <v>0</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="13" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2702,10 +2702,10 @@
       <c r="A9" t="s">
         <v>92</v>
       </c>
-      <c r="B9" s="27">
+      <c r="B9" s="16">
         <v>0</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="13" t="s">
         <v>93</v>
       </c>
     </row>
@@ -2713,10 +2713,10 @@
       <c r="A10" t="s">
         <v>94</v>
       </c>
-      <c r="B10" s="27">
+      <c r="B10" s="16">
         <v>0</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="13" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2724,10 +2724,10 @@
       <c r="A11" t="s">
         <v>95</v>
       </c>
-      <c r="B11" s="27">
+      <c r="B11" s="16">
         <v>9.8000000000000007</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="13" t="s">
         <v>96</v>
       </c>
     </row>
@@ -2735,10 +2735,10 @@
       <c r="A12" t="s">
         <v>97</v>
       </c>
-      <c r="B12" s="27">
+      <c r="B12" s="16">
         <v>1</v>
       </c>
-      <c r="C12" s="33" t="s">
+      <c r="C12" s="22" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2746,10 +2746,10 @@
       <c r="A13" t="s">
         <v>99</v>
       </c>
-      <c r="B13" s="27">
+      <c r="B13" s="16">
         <v>1</v>
       </c>
-      <c r="C13" s="33" t="s">
+      <c r="C13" s="22" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2757,10 +2757,10 @@
       <c r="A14" t="s">
         <v>100</v>
       </c>
-      <c r="B14" s="27">
+      <c r="B14" s="16">
         <v>0</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="13" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2768,10 +2768,10 @@
       <c r="A15" t="s">
         <v>102</v>
       </c>
-      <c r="B15" s="27">
+      <c r="B15" s="16">
         <v>0</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="13" t="s">
         <v>103</v>
       </c>
     </row>
@@ -2779,10 +2779,10 @@
       <c r="A16" t="s">
         <v>104</v>
       </c>
-      <c r="B16" s="27">
+      <c r="B16" s="16">
         <v>40</v>
       </c>
-      <c r="C16" s="24" t="s">
+      <c r="C16" s="13" t="s">
         <v>105</v>
       </c>
     </row>
@@ -2790,10 +2790,10 @@
       <c r="A17" t="s">
         <v>106</v>
       </c>
-      <c r="B17" s="27">
+      <c r="B17" s="16">
         <v>0.5</v>
       </c>
-      <c r="C17" s="24" t="s">
+      <c r="C17" s="13" t="s">
         <v>107</v>
       </c>
     </row>
@@ -2801,10 +2801,10 @@
       <c r="A18" t="s">
         <v>108</v>
       </c>
-      <c r="B18" s="27">
+      <c r="B18" s="16">
         <v>820</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C18" s="13" t="s">
         <v>109</v>
       </c>
     </row>
@@ -2812,10 +2812,10 @@
       <c r="A19" t="s">
         <v>110</v>
       </c>
-      <c r="B19" s="27">
+      <c r="B19" s="16">
         <v>0.05</v>
       </c>
-      <c r="C19" s="24" t="s">
+      <c r="C19" s="13" t="s">
         <v>111</v>
       </c>
     </row>
@@ -2823,10 +2823,10 @@
       <c r="A20" t="s">
         <v>112</v>
       </c>
-      <c r="B20" s="27">
+      <c r="B20" s="16">
         <v>0</v>
       </c>
-      <c r="C20" s="24" t="s">
+      <c r="C20" s="13" t="s">
         <v>113</v>
       </c>
     </row>
@@ -2834,10 +2834,10 @@
       <c r="A21" t="s">
         <v>114</v>
       </c>
-      <c r="B21" s="27">
+      <c r="B21" s="16">
         <v>0.33</v>
       </c>
-      <c r="C21" s="24" t="s">
+      <c r="C21" s="13" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2845,10 +2845,10 @@
       <c r="A22" t="s">
         <v>115</v>
       </c>
-      <c r="B22" s="27">
+      <c r="B22" s="16">
         <v>10</v>
       </c>
-      <c r="C22" s="24" t="s">
+      <c r="C22" s="13" t="s">
         <v>105</v>
       </c>
     </row>
@@ -2856,10 +2856,10 @@
       <c r="A23" t="s">
         <v>116</v>
       </c>
-      <c r="B23" s="27">
+      <c r="B23" s="16">
         <v>1</v>
       </c>
-      <c r="C23" s="24" t="s">
+      <c r="C23" s="13" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2867,10 +2867,10 @@
       <c r="A24" t="s">
         <v>117</v>
       </c>
-      <c r="B24" s="27">
+      <c r="B24" s="16">
         <v>0.1</v>
       </c>
-      <c r="C24" s="24" t="s">
+      <c r="C24" s="13" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2878,10 +2878,10 @@
       <c r="A25" t="s">
         <v>118</v>
       </c>
-      <c r="B25" s="27">
+      <c r="B25" s="16">
         <v>1</v>
       </c>
-      <c r="C25" s="24" t="s">
+      <c r="C25" s="13" t="s">
         <v>98</v>
       </c>
       <c r="D25" t="s">
@@ -2892,10 +2892,10 @@
       <c r="A26" t="s">
         <v>120</v>
       </c>
-      <c r="B26" s="27">
+      <c r="B26" s="16">
         <v>0.5</v>
       </c>
-      <c r="C26" s="24" t="s">
+      <c r="C26" s="13" t="s">
         <v>107</v>
       </c>
     </row>
@@ -2903,10 +2903,10 @@
       <c r="A27" t="s">
         <v>121</v>
       </c>
-      <c r="B27" s="27">
+      <c r="B27" s="16">
         <v>0</v>
       </c>
-      <c r="C27" s="24" t="s">
+      <c r="C27" s="13" t="s">
         <v>109</v>
       </c>
     </row>
@@ -2914,10 +2914,10 @@
       <c r="A28" t="s">
         <v>122</v>
       </c>
-      <c r="B28" s="27">
+      <c r="B28" s="16">
         <v>0</v>
       </c>
-      <c r="C28" s="24" t="s">
+      <c r="C28" s="13" t="s">
         <v>111</v>
       </c>
     </row>
@@ -2925,10 +2925,10 @@
       <c r="A29" t="s">
         <v>123</v>
       </c>
-      <c r="B29" s="27">
+      <c r="B29" s="16">
         <v>0</v>
       </c>
-      <c r="C29" s="24" t="s">
+      <c r="C29" s="13" t="s">
         <v>113</v>
       </c>
     </row>
@@ -2936,10 +2936,10 @@
       <c r="A30" t="s">
         <v>124</v>
       </c>
-      <c r="B30" s="20">
+      <c r="B30" s="9">
         <v>1</v>
       </c>
-      <c r="C30" s="33" t="s">
+      <c r="C30" s="22" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2947,10 +2947,10 @@
       <c r="A31" t="s">
         <v>125</v>
       </c>
-      <c r="B31" s="20">
+      <c r="B31" s="9">
         <v>15</v>
       </c>
-      <c r="C31" s="33" t="s">
+      <c r="C31" s="22" t="s">
         <v>105</v>
       </c>
     </row>
@@ -2958,10 +2958,10 @@
       <c r="A32" t="s">
         <v>126</v>
       </c>
-      <c r="B32" s="27">
+      <c r="B32" s="16">
         <v>1</v>
       </c>
-      <c r="C32" s="24" t="s">
+      <c r="C32" s="13" t="s">
         <v>127</v>
       </c>
     </row>
@@ -2969,10 +2969,10 @@
       <c r="A33" t="s">
         <v>128</v>
       </c>
-      <c r="B33" s="27">
+      <c r="B33" s="16">
         <v>0.08</v>
       </c>
-      <c r="C33" s="24" t="s">
+      <c r="C33" s="13" t="s">
         <v>113</v>
       </c>
     </row>
@@ -2980,10 +2980,10 @@
       <c r="A34" t="s">
         <v>129</v>
       </c>
-      <c r="B34" s="27">
+      <c r="B34" s="16">
         <v>0</v>
       </c>
-      <c r="C34" s="24" t="s">
+      <c r="C34" s="13" t="s">
         <v>130</v>
       </c>
     </row>
@@ -2991,10 +2991,10 @@
       <c r="A35" t="s">
         <v>131</v>
       </c>
-      <c r="B35" s="27">
+      <c r="B35" s="16">
         <v>0</v>
       </c>
-      <c r="C35" s="24" t="s">
+      <c r="C35" s="13" t="s">
         <v>132</v>
       </c>
     </row>
@@ -3002,10 +3002,10 @@
       <c r="A36" t="s">
         <v>133</v>
       </c>
-      <c r="B36" s="27">
+      <c r="B36" s="16">
         <v>40</v>
       </c>
-      <c r="C36" s="24" t="s">
+      <c r="C36" s="13" t="s">
         <v>105</v>
       </c>
     </row>
@@ -3013,10 +3013,10 @@
       <c r="A37" t="s">
         <v>134</v>
       </c>
-      <c r="B37" s="27">
+      <c r="B37" s="16">
         <v>0.05</v>
       </c>
-      <c r="C37" s="24" t="s">
+      <c r="C37" s="13" t="s">
         <v>113</v>
       </c>
     </row>
@@ -3024,10 +3024,10 @@
       <c r="A38" t="s">
         <v>135</v>
       </c>
-      <c r="B38" s="27">
+      <c r="B38" s="16">
         <v>0</v>
       </c>
-      <c r="C38" s="24" t="s">
+      <c r="C38" s="13" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3035,10 +3035,10 @@
       <c r="A39" t="s">
         <v>136</v>
       </c>
-      <c r="B39" s="27">
+      <c r="B39" s="16">
         <v>0</v>
       </c>
-      <c r="C39" s="24" t="s">
+      <c r="C39" s="13" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3046,10 +3046,10 @@
       <c r="A40" t="s">
         <v>137</v>
       </c>
-      <c r="B40" s="27">
+      <c r="B40" s="16">
         <v>1</v>
       </c>
-      <c r="C40" s="24" t="s">
+      <c r="C40" s="13" t="s">
         <v>107</v>
       </c>
     </row>
@@ -3057,10 +3057,10 @@
       <c r="A41" t="s">
         <v>138</v>
       </c>
-      <c r="B41" s="27">
+      <c r="B41" s="16">
         <v>200</v>
       </c>
-      <c r="C41" s="24" t="s">
+      <c r="C41" s="13" t="s">
         <v>109</v>
       </c>
     </row>
@@ -3068,10 +3068,10 @@
       <c r="A42" t="s">
         <v>139</v>
       </c>
-      <c r="B42" s="27">
+      <c r="B42" s="16">
         <v>0</v>
       </c>
-      <c r="C42" s="24" t="s">
+      <c r="C42" s="13" t="s">
         <v>111</v>
       </c>
     </row>
@@ -3079,10 +3079,10 @@
       <c r="A43" t="s">
         <v>140</v>
       </c>
-      <c r="B43" s="27">
+      <c r="B43" s="16">
         <v>0</v>
       </c>
-      <c r="C43" s="24" t="s">
+      <c r="C43" s="13" t="s">
         <v>113</v>
       </c>
     </row>
@@ -3090,10 +3090,10 @@
       <c r="A44" t="s">
         <v>141</v>
       </c>
-      <c r="B44" s="27">
+      <c r="B44" s="16">
         <v>1</v>
       </c>
-      <c r="C44" s="24" t="s">
+      <c r="C44" s="13" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3101,10 +3101,10 @@
       <c r="A45" t="s">
         <v>142</v>
       </c>
-      <c r="B45" s="27">
+      <c r="B45" s="16">
         <v>20</v>
       </c>
-      <c r="C45" s="24" t="s">
+      <c r="C45" s="13" t="s">
         <v>105</v>
       </c>
     </row>
@@ -3112,10 +3112,10 @@
       <c r="A46" t="s">
         <v>143</v>
       </c>
-      <c r="B46" s="27">
+      <c r="B46" s="16">
         <v>1.5</v>
       </c>
-      <c r="C46" s="24" t="s">
+      <c r="C46" s="13" t="s">
         <v>98</v>
       </c>
       <c r="D46" t="s">
@@ -3126,10 +3126,10 @@
       <c r="A47" t="s">
         <v>144</v>
       </c>
-      <c r="B47" s="27">
+      <c r="B47" s="16">
         <v>0.68</v>
       </c>
-      <c r="C47" s="24" t="s">
+      <c r="C47" s="13" t="s">
         <v>145</v>
       </c>
     </row>
@@ -3137,10 +3137,10 @@
       <c r="A48" t="s">
         <v>146</v>
       </c>
-      <c r="B48" s="27">
+      <c r="B48" s="16">
         <v>0.05</v>
       </c>
-      <c r="C48" s="24" t="s">
+      <c r="C48" s="13" t="s">
         <v>147</v>
       </c>
     </row>
@@ -3148,10 +3148,10 @@
       <c r="A49" t="s">
         <v>148</v>
       </c>
-      <c r="B49" s="27">
+      <c r="B49" s="16">
         <v>20000</v>
       </c>
-      <c r="C49" s="24" t="s">
+      <c r="C49" s="13" t="s">
         <v>101</v>
       </c>
     </row>
@@ -3159,10 +3159,10 @@
       <c r="A50" t="s">
         <v>149</v>
       </c>
-      <c r="B50" s="27">
+      <c r="B50" s="16">
         <v>0</v>
       </c>
-      <c r="C50" s="24" t="s">
+      <c r="C50" s="13" t="s">
         <v>103</v>
       </c>
     </row>
@@ -3170,10 +3170,10 @@
       <c r="A51" t="s">
         <v>150</v>
       </c>
-      <c r="B51" s="27">
+      <c r="B51" s="16">
         <v>20</v>
       </c>
-      <c r="C51" s="24" t="s">
+      <c r="C51" s="13" t="s">
         <v>105</v>
       </c>
     </row>
@@ -3181,10 +3181,10 @@
       <c r="A52" t="s">
         <v>151</v>
       </c>
-      <c r="B52" s="27">
+      <c r="B52" s="16">
         <v>0.5</v>
       </c>
-      <c r="C52" s="24" t="s">
+      <c r="C52" s="13" t="s">
         <v>152</v>
       </c>
     </row>
@@ -3192,10 +3192,10 @@
       <c r="A53" t="s">
         <v>153</v>
       </c>
-      <c r="B53" s="27">
+      <c r="B53" s="16">
         <v>1250</v>
       </c>
-      <c r="C53" s="24" t="s">
+      <c r="C53" s="13" t="s">
         <v>154</v>
       </c>
     </row>
@@ -3203,10 +3203,10 @@
       <c r="A54" t="s">
         <v>155</v>
       </c>
-      <c r="B54" s="27">
+      <c r="B54" s="16">
         <v>25</v>
       </c>
-      <c r="C54" s="24" t="s">
+      <c r="C54" s="13" t="s">
         <v>156</v>
       </c>
     </row>
@@ -3214,10 +3214,10 @@
       <c r="A55" t="s">
         <v>157</v>
       </c>
-      <c r="B55" s="27">
+      <c r="B55" s="16">
         <v>0</v>
       </c>
-      <c r="C55" s="24" t="s">
+      <c r="C55" s="13" t="s">
         <v>113</v>
       </c>
     </row>
@@ -3225,10 +3225,10 @@
       <c r="A56" t="s">
         <v>158</v>
       </c>
-      <c r="B56" s="27">
+      <c r="B56" s="16">
         <v>25</v>
       </c>
-      <c r="C56" s="24" t="s">
+      <c r="C56" s="13" t="s">
         <v>105</v>
       </c>
     </row>
@@ -3236,10 +3236,10 @@
       <c r="A57" t="s">
         <v>159</v>
       </c>
-      <c r="B57" s="27">
+      <c r="B57" s="16">
         <v>0.5</v>
       </c>
-      <c r="C57" s="24" t="s">
+      <c r="C57" s="13" t="s">
         <v>107</v>
       </c>
     </row>
@@ -3247,10 +3247,10 @@
       <c r="A58" t="s">
         <v>160</v>
       </c>
-      <c r="B58" s="27">
+      <c r="B58" s="16">
         <v>0</v>
       </c>
-      <c r="C58" s="24" t="s">
+      <c r="C58" s="13" t="s">
         <v>109</v>
       </c>
     </row>
@@ -3258,10 +3258,10 @@
       <c r="A59" t="s">
         <v>161</v>
       </c>
-      <c r="B59" s="27">
+      <c r="B59" s="16">
         <v>0</v>
       </c>
-      <c r="C59" s="24" t="s">
+      <c r="C59" s="13" t="s">
         <v>111</v>
       </c>
     </row>
@@ -3269,10 +3269,10 @@
       <c r="A60" t="s">
         <v>162</v>
       </c>
-      <c r="B60" s="27">
+      <c r="B60" s="16">
         <v>0</v>
       </c>
-      <c r="C60" s="24" t="s">
+      <c r="C60" s="13" t="s">
         <v>113</v>
       </c>
     </row>
@@ -3280,10 +3280,10 @@
       <c r="A61" t="s">
         <v>163</v>
       </c>
-      <c r="B61" s="20">
+      <c r="B61" s="9">
         <v>1</v>
       </c>
-      <c r="C61" s="33" t="s">
+      <c r="C61" s="22" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3291,10 +3291,10 @@
       <c r="A62" t="s">
         <v>164</v>
       </c>
-      <c r="B62" s="20">
+      <c r="B62" s="9">
         <v>15</v>
       </c>
-      <c r="C62" s="33" t="s">
+      <c r="C62" s="22" t="s">
         <v>105</v>
       </c>
     </row>
@@ -3302,10 +3302,10 @@
       <c r="A63" t="s">
         <v>165</v>
       </c>
-      <c r="B63" s="27">
+      <c r="B63" s="16">
         <v>0</v>
       </c>
-      <c r="C63" s="24" t="s">
+      <c r="C63" s="13" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3313,10 +3313,10 @@
       <c r="A64" t="s">
         <v>166</v>
       </c>
-      <c r="B64" s="27">
+      <c r="B64" s="16">
         <v>1</v>
       </c>
-      <c r="C64" s="24" t="s">
+      <c r="C64" s="13" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3324,10 +3324,10 @@
       <c r="A65" t="s">
         <v>167</v>
       </c>
-      <c r="B65" s="27">
+      <c r="B65" s="16">
         <v>0.5</v>
       </c>
-      <c r="C65" s="24" t="s">
+      <c r="C65" s="13" t="s">
         <v>113</v>
       </c>
     </row>
@@ -3335,10 +3335,10 @@
       <c r="A66" t="s">
         <v>168</v>
       </c>
-      <c r="B66" s="27">
+      <c r="B66" s="16">
         <v>0.2</v>
       </c>
-      <c r="C66" s="24" t="s">
+      <c r="C66" s="13" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3346,10 +3346,10 @@
       <c r="A67" t="s">
         <v>169</v>
       </c>
-      <c r="B67" s="27">
+      <c r="B67" s="16">
         <v>1</v>
       </c>
-      <c r="C67" s="24" t="s">
+      <c r="C67" s="13" t="s">
         <v>170</v>
       </c>
     </row>
@@ -3357,10 +3357,10 @@
       <c r="A68" t="s">
         <v>171</v>
       </c>
-      <c r="B68" s="27">
+      <c r="B68" s="16">
         <v>1</v>
       </c>
-      <c r="C68" s="24" t="s">
+      <c r="C68" s="13" t="s">
         <v>170</v>
       </c>
     </row>
@@ -3368,10 +3368,10 @@
       <c r="A69" t="s">
         <v>172</v>
       </c>
-      <c r="B69" s="27">
+      <c r="B69" s="16">
         <v>250</v>
       </c>
-      <c r="C69" s="24" t="s">
+      <c r="C69" s="13" t="s">
         <v>113</v>
       </c>
     </row>
@@ -3379,10 +3379,10 @@
       <c r="A70" t="s">
         <v>173</v>
       </c>
-      <c r="B70" s="27">
+      <c r="B70" s="16">
         <v>6.75</v>
       </c>
-      <c r="C70" s="24" t="s">
+      <c r="C70" s="13" t="s">
         <v>174</v>
       </c>
     </row>
@@ -3390,10 +3390,10 @@
       <c r="A71" t="s">
         <v>175</v>
       </c>
-      <c r="B71" s="27">
+      <c r="B71" s="16">
         <v>13.5</v>
       </c>
-      <c r="C71" s="24" t="s">
+      <c r="C71" s="13" t="s">
         <v>105</v>
       </c>
     </row>
@@ -3401,10 +3401,10 @@
       <c r="A72" t="s">
         <v>176</v>
       </c>
-      <c r="B72" s="27">
+      <c r="B72" s="16">
         <v>0</v>
       </c>
-      <c r="C72" s="24" t="s">
+      <c r="C72" s="13" t="s">
         <v>105</v>
       </c>
     </row>
@@ -3412,10 +3412,10 @@
       <c r="A73" t="s">
         <v>177</v>
       </c>
-      <c r="B73" s="27">
+      <c r="B73" s="16">
         <v>1</v>
       </c>
-      <c r="C73" s="24" t="s">
+      <c r="C73" s="13" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3423,10 +3423,10 @@
       <c r="A74" t="s">
         <v>178</v>
       </c>
-      <c r="B74" s="37">
+      <c r="B74" s="26">
         <v>0.5</v>
       </c>
-      <c r="C74" s="24" t="s">
+      <c r="C74" s="13" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3434,10 +3434,10 @@
       <c r="A75" t="s">
         <v>179</v>
       </c>
-      <c r="B75" s="27">
+      <c r="B75" s="16">
         <v>0.97</v>
       </c>
-      <c r="C75" s="24" t="s">
+      <c r="C75" s="13" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3445,10 +3445,10 @@
       <c r="A76" t="s">
         <v>180</v>
       </c>
-      <c r="B76" s="27">
+      <c r="B76" s="16">
         <v>0.97</v>
       </c>
-      <c r="C76" s="24" t="s">
+      <c r="C76" s="13" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3456,10 +3456,10 @@
       <c r="A77" t="s">
         <v>181</v>
       </c>
-      <c r="B77" s="27">
+      <c r="B77" s="16">
         <v>0</v>
       </c>
-      <c r="C77" s="24" t="s">
+      <c r="C77" s="13" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3467,10 +3467,10 @@
       <c r="A78" t="s">
         <v>182</v>
       </c>
-      <c r="B78" s="27">
+      <c r="B78" s="16">
         <v>500</v>
       </c>
-      <c r="C78" s="24" t="s">
+      <c r="C78" s="13" t="s">
         <v>109</v>
       </c>
     </row>
@@ -3478,10 +3478,10 @@
       <c r="A79" t="s">
         <v>183</v>
       </c>
-      <c r="B79" s="27">
+      <c r="B79" s="16">
         <v>0</v>
       </c>
-      <c r="C79" s="24" t="s">
+      <c r="C79" s="13" t="s">
         <v>111</v>
       </c>
     </row>
@@ -3489,10 +3489,10 @@
       <c r="A80" t="s">
         <v>184</v>
       </c>
-      <c r="B80" s="27">
+      <c r="B80" s="16">
         <v>13.5</v>
       </c>
-      <c r="C80" s="24" t="s">
+      <c r="C80" s="13" t="s">
         <v>105</v>
       </c>
     </row>
@@ -3500,10 +3500,10 @@
       <c r="A81" t="s">
         <v>185</v>
       </c>
-      <c r="B81" s="27" t="s">
+      <c r="B81" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="C81" s="24" t="s">
+      <c r="C81" s="13" t="s">
         <v>187</v>
       </c>
     </row>
@@ -3511,10 +3511,10 @@
       <c r="A82" t="s">
         <v>188</v>
       </c>
-      <c r="B82" s="27">
+      <c r="B82" s="16">
         <v>1</v>
       </c>
-      <c r="C82" s="24" t="s">
+      <c r="C82" s="13" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3522,10 +3522,10 @@
       <c r="A83" t="s">
         <v>189</v>
       </c>
-      <c r="B83" s="27">
+      <c r="B83" s="16">
         <v>0.2</v>
       </c>
-      <c r="C83" s="24" t="s">
+      <c r="C83" s="13" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3533,10 +3533,10 @@
       <c r="A84" t="s">
         <v>190</v>
       </c>
-      <c r="B84" s="27">
+      <c r="B84" s="16">
         <v>0</v>
       </c>
-      <c r="C84" s="24" t="s">
+      <c r="C84" s="13" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3544,10 +3544,10 @@
       <c r="A85" t="s">
         <v>191</v>
       </c>
-      <c r="B85" s="27">
+      <c r="B85" s="16">
         <v>0.16</v>
       </c>
-      <c r="C85" s="24" t="s">
+      <c r="C85" s="13" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3555,10 +3555,10 @@
       <c r="A86" t="s">
         <v>192</v>
       </c>
-      <c r="B86" s="27">
+      <c r="B86" s="16">
         <v>0</v>
       </c>
-      <c r="C86" s="24" t="s">
+      <c r="C86" s="13" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3566,10 +3566,10 @@
       <c r="A87" t="s">
         <v>193</v>
       </c>
-      <c r="B87" s="27">
+      <c r="B87" s="16">
         <v>0</v>
       </c>
-      <c r="C87" s="24" t="s">
+      <c r="C87" s="13" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3577,10 +3577,10 @@
       <c r="A88" t="s">
         <v>194</v>
       </c>
-      <c r="B88" s="27">
+      <c r="B88" s="16">
         <v>0</v>
       </c>
-      <c r="C88" s="24" t="s">
+      <c r="C88" s="13" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3588,10 +3588,10 @@
       <c r="A89" t="s">
         <v>195</v>
       </c>
-      <c r="B89" s="27">
+      <c r="B89" s="16">
         <v>0.5</v>
       </c>
-      <c r="C89" s="24" t="s">
+      <c r="C89" s="13" t="s">
         <v>107</v>
       </c>
     </row>
@@ -3599,10 +3599,10 @@
       <c r="A90" t="s">
         <v>196</v>
       </c>
-      <c r="B90" s="27">
+      <c r="B90" s="16">
         <v>1100</v>
       </c>
-      <c r="C90" s="24" t="s">
+      <c r="C90" s="13" t="s">
         <v>109</v>
       </c>
     </row>
@@ -3610,10 +3610,10 @@
       <c r="A91" t="s">
         <v>197</v>
       </c>
-      <c r="B91" s="27">
+      <c r="B91" s="16">
         <v>0</v>
       </c>
-      <c r="C91" s="24" t="s">
+      <c r="C91" s="13" t="s">
         <v>111</v>
       </c>
     </row>
@@ -3621,10 +3621,10 @@
       <c r="A92" t="s">
         <v>198</v>
       </c>
-      <c r="B92" s="27">
+      <c r="B92" s="16">
         <v>0</v>
       </c>
-      <c r="C92" s="24" t="s">
+      <c r="C92" s="13" t="s">
         <v>113</v>
       </c>
     </row>
@@ -3632,10 +3632,10 @@
       <c r="A93" t="s">
         <v>199</v>
       </c>
-      <c r="B93" s="27">
+      <c r="B93" s="16">
         <v>20</v>
       </c>
-      <c r="C93" s="24" t="s">
+      <c r="C93" s="13" t="s">
         <v>105</v>
       </c>
     </row>
@@ -3643,10 +3643,10 @@
       <c r="A94" t="s">
         <v>200</v>
       </c>
-      <c r="B94" s="20">
+      <c r="B94" s="9">
         <v>2.68</v>
       </c>
-      <c r="C94" s="33" t="s">
+      <c r="C94" s="22" t="s">
         <v>201</v>
       </c>
     </row>
@@ -3654,10 +3654,10 @@
       <c r="A95" t="s">
         <v>202</v>
       </c>
-      <c r="B95" s="20">
+      <c r="B95" s="9">
         <v>0.9</v>
       </c>
-      <c r="C95" s="33" t="s">
+      <c r="C95" s="22" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3679,153 +3679,153 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.453125" style="29" customWidth="1"/>
-    <col min="2" max="2" width="9.81640625" style="29" customWidth="1"/>
-    <col min="3" max="4" width="6.90625" style="29" customWidth="1"/>
+    <col min="1" max="1" width="12.453125" style="18" customWidth="1"/>
+    <col min="2" max="2" width="9.81640625" style="18" customWidth="1"/>
+    <col min="3" max="4" width="6.90625" style="18" customWidth="1"/>
     <col min="5" max="6" width="8.54296875" customWidth="1"/>
     <col min="7" max="7" width="8.36328125" customWidth="1"/>
     <col min="8" max="1025" width="8.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
     </row>
     <row r="2" spans="1:7" ht="13" x14ac:dyDescent="0.3">
-      <c r="A2" s="21"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
     </row>
     <row r="3" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="27" t="s">
         <v>205</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="65" t="s">
         <v>206</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
     </row>
     <row r="4" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="65"/>
+      <c r="G4" s="65"/>
     </row>
     <row r="5" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="66" t="s">
         <v>207</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
     </row>
     <row r="6" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="29" t="s">
         <v>208</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="64" t="s">
         <v>209</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="64"/>
     </row>
     <row r="7" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="29" t="s">
         <v>210</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="64" t="s">
         <v>211</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="64"/>
     </row>
     <row r="8" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="29" t="s">
         <v>212</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="64" t="s">
         <v>213</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="64"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="13" t="s">
         <v>210</v>
       </c>
-      <c r="D10" s="29" t="s">
+      <c r="D10" s="18" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="18" t="s">
         <v>153</v>
       </c>
-      <c r="B11" s="29">
+      <c r="B11" s="18">
         <v>1000</v>
       </c>
-      <c r="C11" s="29">
-        <v>1200</v>
-      </c>
-      <c r="D11" s="29">
+      <c r="C11" s="18">
+        <v>1000</v>
+      </c>
+      <c r="D11" s="18">
         <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="18" t="s">
         <v>158</v>
       </c>
-      <c r="B12" s="29">
-        <v>15</v>
-      </c>
-      <c r="C12" s="29">
-        <v>25</v>
-      </c>
-      <c r="D12" s="29">
+      <c r="B12" s="18">
+        <v>20</v>
+      </c>
+      <c r="C12" s="18">
+        <v>20</v>
+      </c>
+      <c r="D12" s="18">
         <v>5</v>
       </c>
     </row>
@@ -3857,237 +3857,237 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.54296875" style="29" customWidth="1"/>
-    <col min="2" max="2" width="14.453125" style="29" customWidth="1"/>
-    <col min="3" max="3" width="9.1796875" style="29" customWidth="1"/>
-    <col min="4" max="5" width="15" style="29" customWidth="1"/>
-    <col min="6" max="7" width="9.36328125" style="29" customWidth="1"/>
-    <col min="8" max="8" width="8.7265625" style="29" customWidth="1"/>
-    <col min="9" max="9" width="9.36328125" style="29" customWidth="1"/>
-    <col min="10" max="18" width="6.90625" style="29" customWidth="1"/>
-    <col min="19" max="19" width="12.453125" style="29" customWidth="1"/>
-    <col min="20" max="20" width="11.08984375" style="29" customWidth="1"/>
-    <col min="21" max="1023" width="6.90625" style="29" customWidth="1"/>
+    <col min="1" max="1" width="15.54296875" style="18" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" style="18" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" style="18" customWidth="1"/>
+    <col min="4" max="5" width="15" style="18" customWidth="1"/>
+    <col min="6" max="7" width="9.36328125" style="18" customWidth="1"/>
+    <col min="8" max="8" width="8.7265625" style="18" customWidth="1"/>
+    <col min="9" max="9" width="9.36328125" style="18" customWidth="1"/>
+    <col min="10" max="18" width="6.90625" style="18" customWidth="1"/>
+    <col min="19" max="19" width="12.453125" style="18" customWidth="1"/>
+    <col min="20" max="20" width="11.08984375" style="18" customWidth="1"/>
+    <col min="21" max="1023" width="6.90625" style="18" customWidth="1"/>
     <col min="1024" max="1025" width="6.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="I1" s="20"/>
-      <c r="J1" s="24"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="13"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I2" s="20"/>
-      <c r="J2" s="24"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="13"/>
     </row>
     <row r="3" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="27" t="s">
         <v>215</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="65" t="s">
         <v>216</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="24"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="13"/>
     </row>
     <row r="4" spans="1:12" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="27" t="s">
         <v>217</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="65" t="s">
         <v>218</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="24"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="13"/>
     </row>
     <row r="5" spans="1:12" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="27" t="s">
         <v>219</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="65" t="s">
         <v>220</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="24"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="13"/>
     </row>
     <row r="6" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="64" t="s">
         <v>222</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="24"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="24"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="13"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="13"/>
     </row>
     <row r="7" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="11" t="s">
         <v>223</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="64" t="s">
         <v>224</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="24"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="24"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="13"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="13"/>
     </row>
     <row r="8" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="11" t="s">
         <v>225</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="64" t="s">
         <v>226</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="24"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="24"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="13"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="13"/>
     </row>
     <row r="9" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="11" t="s">
         <v>227</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="64" t="s">
         <v>228</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="24"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="24"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="13"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="13"/>
     </row>
     <row r="10" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="64" t="s">
         <v>230</v>
       </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="24"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="24"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="64"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="13"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="13"/>
     </row>
     <row r="11" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="11" t="s">
         <v>231</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="64" t="s">
         <v>232</v>
       </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="24"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="24"/>
+      <c r="C11" s="64"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="13"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="13"/>
     </row>
     <row r="12" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="11" t="s">
         <v>233</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="64" t="s">
         <v>234</v>
       </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="24"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="24"/>
+      <c r="C12" s="64"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="13"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="13"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I13" s="20"/>
-      <c r="J13" s="24"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="13"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="18" t="s">
         <v>235</v>
       </c>
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="18" t="s">
         <v>221</v>
       </c>
-      <c r="C14" s="29" t="s">
+      <c r="C14" s="18" t="s">
         <v>223</v>
       </c>
-      <c r="D14" s="29" t="s">
+      <c r="D14" s="18" t="s">
         <v>236</v>
       </c>
-      <c r="E14" s="29" t="s">
+      <c r="E14" s="18" t="s">
         <v>237</v>
       </c>
-      <c r="F14" s="29" t="s">
+      <c r="F14" s="18" t="s">
         <v>227</v>
       </c>
-      <c r="G14" s="29" t="s">
+      <c r="G14" s="18" t="s">
         <v>229</v>
       </c>
-      <c r="H14" s="29" t="s">
+      <c r="H14" s="18" t="s">
         <v>231</v>
       </c>
-      <c r="I14" s="29" t="s">
+      <c r="I14" s="18" t="s">
         <v>233</v>
       </c>
-      <c r="L14" s="25"/>
+      <c r="L14" s="14"/>
     </row>
     <row r="15" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="18" t="s">
         <v>238</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="18" t="s">
         <v>239</v>
       </c>
-      <c r="C15" s="29" t="s">
+      <c r="C15" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="D15" s="29" t="s">
+      <c r="D15" s="18" t="s">
         <v>240</v>
       </c>
-      <c r="E15" s="29" t="s">
+      <c r="E15" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="F15" s="29" t="s">
+      <c r="F15" s="18" t="s">
         <v>241</v>
       </c>
-      <c r="G15" s="29" t="s">
+      <c r="G15" s="18" t="s">
         <v>242</v>
       </c>
-      <c r="H15" s="29" t="s">
+      <c r="H15" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="I15" s="29" t="s">
+      <c r="I15" s="18" t="s">
         <v>243</v>
       </c>
     </row>
@@ -4118,528 +4118,528 @@
   <dimension ref="A1:AMD38"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.6328125" customWidth="1"/>
-    <col min="2" max="4" width="13.08984375" style="29" customWidth="1"/>
-    <col min="5" max="1018" width="6.90625" style="29" customWidth="1"/>
+    <col min="2" max="4" width="13.08984375" style="18" customWidth="1"/>
+    <col min="5" max="1018" width="6.90625" style="18" customWidth="1"/>
     <col min="1019" max="1025" width="11.54296875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="10" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="41"/>
+      <c r="A2" s="30"/>
     </row>
     <row r="3" spans="1:5" ht="23.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="27" t="s">
         <v>244</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="65" t="s">
         <v>245</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="42"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="31"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="32" t="s">
         <v>246</v>
       </c>
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="32" t="s">
         <v>247</v>
       </c>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="32" t="s">
         <v>248</v>
       </c>
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="32" t="s">
         <v>249</v>
       </c>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="32" t="s">
         <v>250</v>
       </c>
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="32" t="s">
         <v>251</v>
       </c>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="32" t="s">
         <v>252</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="32" t="s">
         <v>251</v>
       </c>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="43" t="s">
+      <c r="A8" s="32" t="s">
         <v>253</v>
       </c>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="32" t="s">
         <v>251</v>
       </c>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="32" t="s">
         <v>254</v>
       </c>
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="32" t="s">
         <v>251</v>
       </c>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="32" t="s">
         <v>255</v>
       </c>
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="32" t="s">
         <v>251</v>
       </c>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="43" t="s">
+      <c r="A11" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="32" t="s">
         <v>256</v>
       </c>
-      <c r="C11" s="44"/>
-      <c r="D11" s="44"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="32" t="s">
         <v>257</v>
       </c>
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="32" t="s">
         <v>258</v>
       </c>
-      <c r="C12" s="44"/>
-      <c r="D12" s="44"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="32" t="s">
         <v>259</v>
       </c>
-      <c r="B13" s="43" t="s">
+      <c r="B13" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="C13" s="44"/>
-      <c r="D13" s="44"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="43" t="s">
+      <c r="A14" s="32" t="s">
         <v>261</v>
       </c>
-      <c r="B14" s="43" t="s">
+      <c r="B14" s="32" t="s">
         <v>262</v>
       </c>
-      <c r="C14" s="44"/>
-      <c r="D14" s="44"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="43" t="s">
+      <c r="A15" s="32" t="s">
         <v>263</v>
       </c>
-      <c r="B15" s="43" t="s">
+      <c r="B15" s="32" t="s">
         <v>264</v>
       </c>
-      <c r="C15" s="44"/>
-      <c r="D15" s="44"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
     </row>
     <row r="17" spans="1:5" ht="123" x14ac:dyDescent="0.25">
-      <c r="A17" s="45" t="s">
+      <c r="A17" s="34" t="s">
         <v>246</v>
       </c>
-      <c r="B17" s="46" t="s">
+      <c r="B17" s="35" t="s">
         <v>265</v>
       </c>
-      <c r="C17" s="46" t="s">
+      <c r="C17" s="35" t="s">
         <v>266</v>
       </c>
-      <c r="D17" s="46" t="s">
+      <c r="D17" s="35" t="s">
         <v>267</v>
       </c>
-      <c r="E17" s="46" t="s">
+      <c r="E17" s="35" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="45" t="s">
+      <c r="A18" s="34" t="s">
         <v>269</v>
       </c>
-      <c r="B18" s="47" t="s">
+      <c r="B18" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="47" t="s">
+      <c r="C18" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="47" t="s">
+      <c r="D18" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="E18" s="47" t="s">
+      <c r="E18" s="36" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="45" t="s">
+      <c r="A19" s="34" t="s">
         <v>248</v>
       </c>
-      <c r="B19" s="47" t="s">
+      <c r="B19" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="47" t="s">
+      <c r="C19" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="47" t="s">
+      <c r="D19" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="E19" s="47" t="s">
+      <c r="E19" s="36" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="45" t="s">
+      <c r="A20" s="34" t="s">
         <v>270</v>
       </c>
-      <c r="B20" s="47" t="s">
+      <c r="B20" s="36" t="s">
         <v>186</v>
       </c>
-      <c r="C20" s="47" t="s">
+      <c r="C20" s="36" t="s">
         <v>271</v>
       </c>
-      <c r="D20" s="47" t="s">
+      <c r="D20" s="36" t="s">
         <v>271</v>
       </c>
-      <c r="E20" s="47" t="s">
+      <c r="E20" s="36" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="45" t="s">
+      <c r="A21" s="34" t="s">
         <v>272</v>
       </c>
-      <c r="B21" s="47" t="s">
+      <c r="B21" s="36" t="s">
         <v>186</v>
       </c>
-      <c r="C21" s="47" t="s">
+      <c r="C21" s="36" t="s">
         <v>186</v>
       </c>
-      <c r="D21" s="47" t="s">
+      <c r="D21" s="36" t="s">
         <v>186</v>
       </c>
-      <c r="E21" s="47" t="s">
+      <c r="E21" s="36" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="45" t="s">
+      <c r="A22" s="34" t="s">
         <v>273</v>
       </c>
-      <c r="B22" s="47" t="s">
+      <c r="B22" s="36" t="s">
         <v>186</v>
       </c>
-      <c r="C22" s="47" t="s">
+      <c r="C22" s="36" t="s">
         <v>186</v>
       </c>
-      <c r="D22" s="47" t="s">
+      <c r="D22" s="36" t="s">
         <v>271</v>
       </c>
-      <c r="E22" s="47" t="s">
+      <c r="E22" s="36" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="48" t="s">
+      <c r="A23" s="37" t="s">
         <v>274</v>
       </c>
-      <c r="B23" s="47" t="s">
+      <c r="B23" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="47" t="s">
+      <c r="C23" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="47" t="s">
+      <c r="D23" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="E23" s="47" t="s">
+      <c r="E23" s="36" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="48" t="s">
+      <c r="A24" s="37" t="s">
         <v>275</v>
       </c>
-      <c r="B24" s="47" t="s">
+      <c r="B24" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="C24" s="47" t="s">
+      <c r="C24" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="D24" s="47" t="s">
+      <c r="D24" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="E24" s="47" t="s">
+      <c r="E24" s="36" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="45" t="s">
+      <c r="A25" s="34" t="s">
         <v>276</v>
       </c>
-      <c r="B25" s="47" t="s">
+      <c r="B25" s="36" t="s">
         <v>271</v>
       </c>
-      <c r="C25" s="47" t="s">
+      <c r="C25" s="36" t="s">
         <v>271</v>
       </c>
-      <c r="D25" s="47" t="s">
+      <c r="D25" s="36" t="s">
         <v>271</v>
       </c>
-      <c r="E25" s="47" t="s">
+      <c r="E25" s="36" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="45" t="s">
+      <c r="A26" s="34" t="s">
         <v>277</v>
       </c>
-      <c r="B26" s="47" t="s">
+      <c r="B26" s="36" t="s">
         <v>271</v>
       </c>
-      <c r="C26" s="47" t="s">
+      <c r="C26" s="36" t="s">
         <v>271</v>
       </c>
-      <c r="D26" s="47" t="s">
+      <c r="D26" s="36" t="s">
         <v>271</v>
       </c>
-      <c r="E26" s="47" t="s">
+      <c r="E26" s="36" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="48" t="s">
+      <c r="A27" s="37" t="s">
         <v>278</v>
       </c>
-      <c r="B27" s="47" t="s">
+      <c r="B27" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="47" t="s">
+      <c r="C27" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="D27" s="47" t="s">
+      <c r="D27" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="E27" s="47" t="s">
+      <c r="E27" s="36" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="45" t="s">
+      <c r="A28" s="34" t="s">
         <v>279</v>
       </c>
-      <c r="B28" s="47" t="s">
+      <c r="B28" s="36" t="s">
         <v>271</v>
       </c>
-      <c r="C28" s="47" t="s">
+      <c r="C28" s="36" t="s">
         <v>271</v>
       </c>
-      <c r="D28" s="47" t="s">
+      <c r="D28" s="36" t="s">
         <v>271</v>
       </c>
-      <c r="E28" s="47" t="s">
+      <c r="E28" s="36" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="48" t="s">
+      <c r="A29" s="37" t="s">
         <v>280</v>
       </c>
-      <c r="B29" s="47" t="s">
+      <c r="B29" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="47" t="s">
+      <c r="C29" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="D29" s="47" t="s">
+      <c r="D29" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="E29" s="47" t="s">
+      <c r="E29" s="36" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="48" t="s">
+      <c r="A30" s="37" t="s">
         <v>281</v>
       </c>
-      <c r="B30" s="47" t="s">
+      <c r="B30" s="36" t="s">
         <v>282</v>
       </c>
-      <c r="C30" s="47" t="s">
+      <c r="C30" s="36" t="s">
         <v>282</v>
       </c>
-      <c r="D30" s="47" t="s">
+      <c r="D30" s="36" t="s">
         <v>282</v>
       </c>
-      <c r="E30" s="47" t="s">
+      <c r="E30" s="36" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="45" t="s">
+      <c r="A31" s="34" t="s">
         <v>283</v>
       </c>
-      <c r="B31" s="47" t="s">
+      <c r="B31" s="36" t="s">
         <v>186</v>
       </c>
-      <c r="C31" s="47" t="s">
+      <c r="C31" s="36" t="s">
         <v>186</v>
       </c>
-      <c r="D31" s="47" t="s">
+      <c r="D31" s="36" t="s">
         <v>186</v>
       </c>
-      <c r="E31" s="47" t="s">
+      <c r="E31" s="36" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="45" t="s">
+      <c r="A32" s="34" t="s">
         <v>284</v>
       </c>
-      <c r="B32" s="47" t="s">
+      <c r="B32" s="36" t="s">
         <v>186</v>
       </c>
-      <c r="C32" s="47" t="s">
+      <c r="C32" s="36" t="s">
         <v>186</v>
       </c>
-      <c r="D32" s="47" t="s">
+      <c r="D32" s="36" t="s">
         <v>186</v>
       </c>
-      <c r="E32" s="47" t="s">
+      <c r="E32" s="36" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="45" t="s">
+      <c r="A33" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="B33" s="47" t="s">
+      <c r="B33" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="47" t="s">
+      <c r="C33" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="D33" s="47" t="s">
+      <c r="D33" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="E33" s="47" t="s">
+      <c r="E33" s="36" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="45" t="s">
+      <c r="A34" s="34" t="s">
         <v>257</v>
       </c>
-      <c r="B34" s="47" t="s">
+      <c r="B34" s="36" t="s">
         <v>285</v>
       </c>
-      <c r="C34" s="47" t="s">
+      <c r="C34" s="36" t="s">
         <v>285</v>
       </c>
-      <c r="D34" s="47" t="s">
+      <c r="D34" s="36" t="s">
         <v>285</v>
       </c>
-      <c r="E34" s="47" t="s">
+      <c r="E34" s="36" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="45" t="s">
+      <c r="A35" s="34" t="s">
         <v>259</v>
       </c>
-      <c r="B35" s="47" t="s">
+      <c r="B35" s="36" t="s">
         <v>286</v>
       </c>
-      <c r="C35" s="47" t="s">
+      <c r="C35" s="36" t="s">
         <v>286</v>
       </c>
-      <c r="D35" s="47" t="s">
+      <c r="D35" s="36" t="s">
         <v>286</v>
       </c>
-      <c r="E35" s="47" t="s">
+      <c r="E35" s="36" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="45" t="s">
+      <c r="A36" s="34" t="s">
         <v>261</v>
       </c>
-      <c r="B36" s="47" t="s">
+      <c r="B36" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="C36" s="47" t="s">
+      <c r="C36" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="D36" s="47" t="s">
+      <c r="D36" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="E36" s="47" t="s">
+      <c r="E36" s="36" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="45" t="s">
+      <c r="A37" s="34" t="s">
         <v>263</v>
       </c>
-      <c r="B37" s="47" t="s">
+      <c r="B37" s="36" t="s">
         <v>186</v>
       </c>
-      <c r="C37" s="47" t="s">
+      <c r="C37" s="36" t="s">
         <v>186</v>
       </c>
-      <c r="D37" s="47" t="s">
+      <c r="D37" s="36" t="s">
         <v>186</v>
       </c>
-      <c r="E37" s="47" t="s">
+      <c r="E37" s="36" t="s">
         <v>186</v>
       </c>
-      <c r="F37" s="47"/>
+      <c r="F37" s="36"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="45" t="s">
+      <c r="A38" s="34" t="s">
         <v>287</v>
       </c>
-      <c r="B38" s="49" t="s">
+      <c r="B38" s="38" t="s">
         <v>288</v>
       </c>
-      <c r="C38" s="49" t="s">
+      <c r="C38" s="38" t="s">
         <v>288</v>
       </c>
-      <c r="D38" s="49" t="s">
+      <c r="D38" s="38" t="s">
         <v>288</v>
       </c>
-      <c r="E38" s="49" t="s">
+      <c r="E38" s="38" t="s">
         <v>288</v>
       </c>
     </row>
@@ -4678,509 +4678,509 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="39" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="50"/>
+      <c r="A2" s="39"/>
     </row>
     <row r="3" spans="1:8" ht="23.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="27" t="s">
         <v>290</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="65" t="s">
         <v>291</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="32" t="s">
         <v>292</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="67" t="s">
         <v>293</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="32" t="s">
         <v>294</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="67" t="s">
         <v>295</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67"/>
     </row>
     <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="51" t="s">
+      <c r="A6" s="40" t="s">
         <v>296</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="65" t="s">
         <v>297</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="65"/>
+      <c r="H6" s="65"/>
     </row>
     <row r="7" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="51" t="s">
+      <c r="A7" s="40" t="s">
         <v>298</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="65" t="s">
         <v>299</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="65"/>
     </row>
     <row r="8" spans="1:8" ht="41" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="51" t="s">
+      <c r="A8" s="40" t="s">
         <v>300</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="65" t="s">
         <v>301</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
+      <c r="C8" s="65"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="65"/>
+      <c r="G8" s="65"/>
+      <c r="H8" s="65"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="52" t="s">
+      <c r="A10" s="41" t="s">
         <v>302</v>
       </c>
-      <c r="B10" s="53" t="s">
+      <c r="B10" s="42" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="54" t="s">
+      <c r="A11" s="43" t="s">
         <v>304</v>
       </c>
-      <c r="B11" s="54">
+      <c r="B11" s="43">
         <v>0.28622953868737899</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="54" t="s">
+      <c r="A12" s="43" t="s">
         <v>305</v>
       </c>
-      <c r="B12" s="54">
+      <c r="B12" s="43">
         <v>0.25807310904584102</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="54" t="s">
+      <c r="A13" s="43" t="s">
         <v>306</v>
       </c>
-      <c r="B13" s="54">
+      <c r="B13" s="43">
         <v>0.23396226376115001</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="54" t="s">
+      <c r="A14" s="43" t="s">
         <v>307</v>
       </c>
-      <c r="B14" s="54">
+      <c r="B14" s="43">
         <v>0.22173508850563001</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="70" t="s">
         <v>308</v>
       </c>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
+      <c r="F16" s="70"/>
+      <c r="G16" s="70"/>
+      <c r="H16" s="70"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="56" t="s">
+      <c r="A17" s="45" t="s">
         <v>302</v>
       </c>
-      <c r="B17" s="56" t="s">
+      <c r="B17" s="45" t="s">
         <v>309</v>
       </c>
-      <c r="C17" s="57" t="s">
+      <c r="C17" s="46" t="s">
         <v>294</v>
       </c>
-      <c r="D17" s="58" t="s">
+      <c r="D17" s="47" t="s">
         <v>303</v>
       </c>
-      <c r="E17" s="55" t="s">
+      <c r="E17" s="44" t="s">
         <v>310</v>
       </c>
-      <c r="F17" s="55" t="s">
+      <c r="F17" s="44" t="s">
         <v>311</v>
       </c>
-      <c r="G17" s="55" t="s">
+      <c r="G17" s="44" t="s">
         <v>312</v>
       </c>
-      <c r="H17" s="55" t="s">
+      <c r="H17" s="44" t="s">
         <v>313</v>
       </c>
-      <c r="I17" s="55" t="s">
+      <c r="I17" s="44" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="71" t="s">
         <v>315</v>
       </c>
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="48" t="s">
         <v>316</v>
       </c>
-      <c r="C18" s="60" t="s">
+      <c r="C18" s="49" t="s">
         <v>317</v>
       </c>
-      <c r="D18" s="61">
+      <c r="D18" s="50">
         <v>0.51388888888888895</v>
       </c>
-      <c r="E18" s="62"/>
-      <c r="F18" s="55"/>
-      <c r="G18" s="55"/>
-      <c r="H18" s="55"/>
-      <c r="I18" s="63" t="s">
+      <c r="E18" s="51"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="44"/>
+      <c r="H18" s="44"/>
+      <c r="I18" s="52" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="64" t="s">
+      <c r="A19" s="71"/>
+      <c r="B19" s="53" t="s">
         <v>319</v>
       </c>
-      <c r="C19" s="65" t="s">
+      <c r="C19" s="54" t="s">
         <v>320</v>
       </c>
-      <c r="D19" s="66">
+      <c r="D19" s="55">
         <v>0.48611111111111099</v>
       </c>
-      <c r="E19" s="62"/>
-      <c r="F19" s="55"/>
-      <c r="G19" s="55"/>
-      <c r="H19" s="55"/>
-      <c r="I19" s="63" t="s">
+      <c r="E19" s="51"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="44"/>
+      <c r="I19" s="52" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="71" t="s">
         <v>321</v>
       </c>
-      <c r="B20" s="59" t="s">
+      <c r="B20" s="48" t="s">
         <v>322</v>
       </c>
-      <c r="C20" s="60" t="s">
+      <c r="C20" s="49" t="s">
         <v>323</v>
       </c>
-      <c r="D20" s="61">
+      <c r="D20" s="50">
         <v>0.25987103174603199</v>
       </c>
-      <c r="E20" s="62"/>
-      <c r="F20" s="55"/>
-      <c r="G20" s="55"/>
-      <c r="H20" s="55"/>
-      <c r="I20" s="63" t="s">
+      <c r="E20" s="51"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="52" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="67" t="s">
+      <c r="A21" s="71"/>
+      <c r="B21" s="56" t="s">
         <v>324</v>
       </c>
-      <c r="C21" s="54" t="s">
+      <c r="C21" s="43" t="s">
         <v>325</v>
       </c>
-      <c r="D21" s="68">
+      <c r="D21" s="57">
         <v>0.23849206349206301</v>
       </c>
-      <c r="E21" s="62"/>
-      <c r="F21" s="55"/>
-      <c r="G21" s="55"/>
-      <c r="H21" s="55"/>
-      <c r="I21" s="63" t="s">
+      <c r="E21" s="51"/>
+      <c r="F21" s="44"/>
+      <c r="G21" s="44"/>
+      <c r="H21" s="44"/>
+      <c r="I21" s="52" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="67" t="s">
+      <c r="A22" s="71"/>
+      <c r="B22" s="56" t="s">
         <v>326</v>
       </c>
-      <c r="C22" s="54" t="s">
+      <c r="C22" s="43" t="s">
         <v>327</v>
       </c>
-      <c r="D22" s="68">
+      <c r="D22" s="57">
         <v>0.246825396825397</v>
       </c>
-      <c r="E22" s="69">
+      <c r="E22" s="58">
         <v>2.75</v>
       </c>
-      <c r="F22" s="63" t="s">
+      <c r="F22" s="52" t="s">
         <v>186</v>
       </c>
-      <c r="G22" s="63">
+      <c r="G22" s="52">
         <v>1.88</v>
       </c>
-      <c r="H22" s="63">
+      <c r="H22" s="52">
         <v>3</v>
       </c>
-      <c r="I22" s="63" t="s">
+      <c r="I22" s="52" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="64" t="s">
+      <c r="A23" s="71"/>
+      <c r="B23" s="53" t="s">
         <v>328</v>
       </c>
-      <c r="C23" s="65" t="s">
+      <c r="C23" s="54" t="s">
         <v>329</v>
       </c>
-      <c r="D23" s="66">
+      <c r="D23" s="55">
         <v>0.25481150793650797</v>
       </c>
-      <c r="E23" s="69">
+      <c r="E23" s="58">
         <v>2.25</v>
       </c>
-      <c r="F23" s="63" t="s">
+      <c r="F23" s="52" t="s">
         <v>186</v>
       </c>
-      <c r="G23" s="63">
+      <c r="G23" s="52">
         <v>1.5</v>
       </c>
-      <c r="H23" s="63">
+      <c r="H23" s="52">
         <v>3</v>
       </c>
-      <c r="I23" s="63" t="s">
+      <c r="I23" s="52" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="72" t="s">
         <v>330</v>
       </c>
-      <c r="B24" s="70" t="s">
+      <c r="B24" s="59" t="s">
         <v>331</v>
       </c>
-      <c r="C24" s="54" t="s">
+      <c r="C24" s="43" t="s">
         <v>332</v>
       </c>
-      <c r="D24" s="68">
+      <c r="D24" s="57">
         <v>0.26535443722943702</v>
       </c>
-      <c r="E24" s="69">
+      <c r="E24" s="58">
         <v>2</v>
       </c>
-      <c r="F24" s="63" t="s">
+      <c r="F24" s="52" t="s">
         <v>186</v>
       </c>
-      <c r="G24" s="63">
+      <c r="G24" s="52">
         <v>2.6</v>
       </c>
-      <c r="H24" s="63">
+      <c r="H24" s="52">
         <v>2.17</v>
       </c>
-      <c r="I24" s="63" t="s">
+      <c r="I24" s="52" t="s">
         <v>333</v>
       </c>
-      <c r="N24" s="2"/>
+      <c r="N24" s="68"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="70" t="s">
+      <c r="A25" s="72"/>
+      <c r="B25" s="59" t="s">
         <v>334</v>
       </c>
-      <c r="C25" s="54" t="s">
+      <c r="C25" s="43" t="s">
         <v>335</v>
       </c>
-      <c r="D25" s="68">
+      <c r="D25" s="57">
         <v>0.39644209956710003</v>
       </c>
-      <c r="E25" s="62"/>
-      <c r="F25" s="55"/>
-      <c r="G25" s="55"/>
-      <c r="H25" s="55"/>
-      <c r="I25" s="63" t="s">
+      <c r="E25" s="51"/>
+      <c r="F25" s="44"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="44"/>
+      <c r="I25" s="52" t="s">
         <v>318</v>
       </c>
-      <c r="N25" s="2"/>
+      <c r="N25" s="68"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="B26" s="71" t="s">
+      <c r="A26" s="72"/>
+      <c r="B26" s="60" t="s">
         <v>336</v>
       </c>
-      <c r="C26" s="65" t="s">
+      <c r="C26" s="54" t="s">
         <v>337</v>
       </c>
-      <c r="D26" s="66">
+      <c r="D26" s="55">
         <v>0.33820346320346301</v>
       </c>
-      <c r="E26" s="69">
+      <c r="E26" s="58">
         <v>2.57</v>
       </c>
-      <c r="F26" s="63" t="s">
+      <c r="F26" s="52" t="s">
         <v>186</v>
       </c>
-      <c r="G26" s="63">
+      <c r="G26" s="52">
         <v>1.71</v>
       </c>
-      <c r="H26" s="63">
+      <c r="H26" s="52">
         <v>2.14</v>
       </c>
-      <c r="I26" s="63" t="s">
+      <c r="I26" s="52" t="s">
         <v>333</v>
       </c>
-      <c r="N26" s="2"/>
+      <c r="N26" s="68"/>
     </row>
     <row r="27" spans="1:14" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="69" t="s">
         <v>338</v>
       </c>
-      <c r="B27" s="72" t="s">
+      <c r="B27" s="61" t="s">
         <v>339</v>
       </c>
-      <c r="C27" s="60" t="s">
+      <c r="C27" s="49" t="s">
         <v>340</v>
       </c>
-      <c r="D27" s="61">
+      <c r="D27" s="50">
         <v>0.25580808080808098</v>
       </c>
-      <c r="E27" s="69">
+      <c r="E27" s="58">
         <v>0</v>
       </c>
-      <c r="F27" s="63" t="s">
+      <c r="F27" s="52" t="s">
         <v>186</v>
       </c>
-      <c r="G27" s="63">
+      <c r="G27" s="52">
         <v>0.77</v>
       </c>
-      <c r="H27" s="63">
+      <c r="H27" s="52">
         <v>0.44</v>
       </c>
-      <c r="I27" s="63" t="s">
+      <c r="I27" s="52" t="s">
         <v>318</v>
       </c>
-      <c r="J27" s="25" t="s">
+      <c r="J27" s="14" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="70" t="s">
+      <c r="A28" s="69"/>
+      <c r="B28" s="59" t="s">
         <v>342</v>
       </c>
-      <c r="C28" s="54" t="s">
+      <c r="C28" s="43" t="s">
         <v>343</v>
       </c>
-      <c r="D28" s="68">
+      <c r="D28" s="57">
         <v>0.38377525252525302</v>
       </c>
-      <c r="E28" s="69">
+      <c r="E28" s="58">
         <v>2.63</v>
       </c>
-      <c r="F28" s="63" t="s">
+      <c r="F28" s="52" t="s">
         <v>186</v>
       </c>
-      <c r="G28" s="63">
+      <c r="G28" s="52">
         <v>1</v>
       </c>
-      <c r="H28" s="63">
+      <c r="H28" s="52">
         <v>1.88</v>
       </c>
-      <c r="I28" s="63" t="s">
+      <c r="I28" s="52" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="71" t="s">
+      <c r="A29" s="69"/>
+      <c r="B29" s="60" t="s">
         <v>344</v>
       </c>
-      <c r="C29" s="65" t="s">
+      <c r="C29" s="54" t="s">
         <v>345</v>
       </c>
-      <c r="D29" s="66">
+      <c r="D29" s="55">
         <v>0.360416666666667</v>
       </c>
-      <c r="E29" s="69">
+      <c r="E29" s="58">
         <v>1.63</v>
       </c>
-      <c r="F29" s="63" t="s">
+      <c r="F29" s="52" t="s">
         <v>186</v>
       </c>
-      <c r="G29" s="63">
+      <c r="G29" s="52">
         <v>1.5</v>
       </c>
-      <c r="H29" s="63">
+      <c r="H29" s="52">
         <v>2.63</v>
       </c>
-      <c r="I29" s="63" t="s">
+      <c r="I29" s="52" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="70" t="s">
         <v>300</v>
       </c>
-      <c r="B32" s="5"/>
+      <c r="B32" s="70"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="55" t="s">
+      <c r="A33" s="44" t="s">
         <v>346</v>
       </c>
-      <c r="B33" s="55" t="s">
+      <c r="B33" s="44" t="s">
         <v>347</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="54" t="str">
+      <c r="A34" s="43" t="str">
         <f>IF(input_sensitivity!A11 = "","",input_sensitivity!A11)</f>
         <v>pv_cost_investment</v>
       </c>
-      <c r="B34" s="54" t="b">
+      <c r="B34" s="43" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="54" t="str">
+      <c r="A35" s="43" t="str">
         <f>IF(input_sensitivity!A12 = "","",input_sensitivity!A12)</f>
         <v>pv_lifetime</v>
       </c>
-      <c r="B35" s="54" t="b">
+      <c r="B35" s="43" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Changed input files for critical demand
</commit_message>
<xml_diff>
--- a/inputs/test_input_template.xlsx
+++ b/inputs/test_input_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="351">
   <si>
     <t xml:space="preserve">Tool for optimizing and simulating off- and on-grid electrification solutions</t>
   </si>
@@ -742,16 +742,25 @@
     <t xml:space="preserve">title_demand_ac</t>
   </si>
   <si>
+    <t xml:space="preserve">title_demand_ac_critical</t>
+  </si>
+  <si>
     <t xml:space="preserve">title_demand_dc</t>
   </si>
   <si>
+    <t xml:space="preserve">title_demand_dc_critical</t>
+  </si>
+  <si>
     <t xml:space="preserve">test_site</t>
   </si>
   <si>
     <t xml:space="preserve">test_site.csv</t>
   </si>
   <si>
-    <t xml:space="preserve">Demand</t>
+    <t xml:space="preserve">demand_ac_critical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">demand_dc_critical</t>
   </si>
   <si>
     <t xml:space="preserve">SolarGen</t>
@@ -892,7 +901,7 @@
     <t xml:space="preserve">default</t>
   </si>
   <si>
-    <t xml:space="preserve">share_hybrid</t>
+    <t xml:space="preserve">critical</t>
   </si>
   <si>
     <t xml:space="preserve">evaluation_perspective</t>
@@ -1106,11 +1115,11 @@
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="DD/MM/YY\ HH:MM"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yy\ hh:mm"/>
     <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="168" formatCode="#,##0.00"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1159,11 +1168,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1354,7 +1358,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="71">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1599,10 +1603,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1645,12 +1645,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1716,7 +1716,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1726,13 +1726,12 @@
       <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="1.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="49.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="1.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.54"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1926,22 +1925,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="18.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2374,23 +2372,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:G95"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A63" activeCellId="0" sqref="A63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="6.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="24" width="6.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="4" style="0" width="8.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="6.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="6.09"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3452,7 +3449,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -3462,14 +3459,12 @@
       <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="20" width="12.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="20" width="9.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="20" width="6.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="8.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3628,42 +3623,41 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C12" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="6.921875" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="20" width="15.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="20" width="14.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="20" width="9.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="20" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="20" width="9.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="20" width="8.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="20" width="9.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="10" style="20" width="6.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="20" width="12.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="20" width="11.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="21" style="20" width="6.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="6.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="4" style="20" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="20" width="9.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="20" width="8.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="20" width="9.36"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="20" min="12" style="20" width="6.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="20" width="12.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="20" width="11.1"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="23" style="20" width="6.91"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="I1" s="10"/>
-      <c r="J1" s="15"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="15"/>
     </row>
     <row r="2" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I2" s="10"/>
-      <c r="J2" s="15"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="15"/>
     </row>
     <row r="3" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="29" t="s">
@@ -3675,11 +3669,13 @@
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
       <c r="E3" s="30"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="15"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="15"/>
     </row>
     <row r="4" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="29" t="s">
@@ -3691,11 +3687,13 @@
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
       <c r="E4" s="30"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="15"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="15"/>
     </row>
     <row r="5" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="29" t="s">
@@ -3707,11 +3705,13 @@
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
       <c r="E5" s="30"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="15"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="15"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="12" t="s">
@@ -3723,9 +3723,11 @@
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
-      <c r="F6" s="15"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="15"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="15"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="15"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="12" t="s">
@@ -3737,9 +3739,11 @@
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
-      <c r="F7" s="15"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="15"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="15"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="15"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="12" t="s">
@@ -3751,9 +3755,11 @@
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
-      <c r="F8" s="15"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="15"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="15"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="15"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="s">
@@ -3765,9 +3771,11 @@
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
-      <c r="F9" s="15"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="15"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="15"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="15"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="12" t="s">
@@ -3779,9 +3787,11 @@
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
-      <c r="F10" s="15"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="15"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="15"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="15"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="12" t="s">
@@ -3793,9 +3803,11 @@
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
-      <c r="F11" s="15"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="15"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="15"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="15"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="12" t="s">
@@ -3807,13 +3819,15 @@
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
-      <c r="F12" s="15"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="15"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="15"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="15"/>
     </row>
     <row r="13" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I13" s="10"/>
-      <c r="J13" s="15"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="15"/>
     </row>
     <row r="14" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="20" t="s">
@@ -3832,46 +3846,58 @@
         <v>238</v>
       </c>
       <c r="F14" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>240</v>
+      </c>
+      <c r="H14" s="20" t="s">
         <v>228</v>
       </c>
-      <c r="G14" s="20" t="s">
+      <c r="I14" s="20" t="s">
         <v>230</v>
       </c>
-      <c r="H14" s="20" t="s">
+      <c r="J14" s="20" t="s">
         <v>232</v>
       </c>
-      <c r="I14" s="20" t="s">
+      <c r="K14" s="20" t="s">
         <v>234</v>
       </c>
-      <c r="L14" s="16"/>
+      <c r="N14" s="16"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="20" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="C15" s="20" t="s">
         <v>187</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>241</v>
+        <v>187</v>
       </c>
       <c r="E15" s="20" t="s">
+        <v>243</v>
+      </c>
+      <c r="F15" s="20" t="s">
         <v>187</v>
       </c>
-      <c r="F15" s="20" t="s">
-        <v>242</v>
-      </c>
       <c r="G15" s="20" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="H15" s="20" t="s">
+        <v>245</v>
+      </c>
+      <c r="I15" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="J15" s="20" t="s">
         <v>187</v>
       </c>
-      <c r="I15" s="20" t="s">
-        <v>244</v>
+      <c r="K15" s="20" t="s">
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -3898,22 +3924,22 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="6.921875" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="20" width="13.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1018" min="5" style="20" width="6.91"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1019" style="0" width="11.54"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1018" min="5" style="20" width="6.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1019" style="0" width="11.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3926,10 +3952,10 @@
     </row>
     <row r="3" customFormat="false" ht="23.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="29" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -3937,70 +3963,70 @@
     </row>
     <row r="4" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="35" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C4" s="36"/>
       <c r="D4" s="36"/>
     </row>
     <row r="5" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="35" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="C5" s="36"/>
       <c r="D5" s="36"/>
     </row>
     <row r="6" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="35" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="C6" s="36"/>
       <c r="D6" s="36"/>
     </row>
     <row r="7" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="35" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="B7" s="35" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="C7" s="36"/>
       <c r="D7" s="36"/>
     </row>
     <row r="8" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="35" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="B8" s="35" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="C8" s="36"/>
       <c r="D8" s="36"/>
     </row>
     <row r="9" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="35" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="B9" s="35" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="C9" s="36"/>
       <c r="D9" s="36"/>
     </row>
     <row r="10" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="35" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="B10" s="35" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="C10" s="36"/>
       <c r="D10" s="36"/>
@@ -4010,71 +4036,71 @@
         <v>42</v>
       </c>
       <c r="B11" s="35" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="C11" s="36"/>
       <c r="D11" s="36"/>
     </row>
     <row r="12" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="35" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="B12" s="35" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="C12" s="36"/>
       <c r="D12" s="36"/>
     </row>
     <row r="13" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="35" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="B13" s="35" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="C13" s="36"/>
       <c r="D13" s="36"/>
     </row>
     <row r="14" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="35" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="B14" s="35" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C14" s="36"/>
       <c r="D14" s="36"/>
     </row>
     <row r="15" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="35" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="B15" s="35" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="C15" s="36"/>
       <c r="D15" s="36"/>
     </row>
-    <row r="17" customFormat="false" ht="123" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="122" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="37" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="B17" s="38" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="C17" s="38" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="D17" s="38" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="E17" s="38" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="37" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="B18" s="39" t="s">
         <v>39</v>
@@ -4091,7 +4117,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="37" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="B19" s="39" t="s">
         <v>39</v>
@@ -4108,24 +4134,24 @@
     </row>
     <row r="20" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="37" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="B20" s="39" t="s">
         <v>187</v>
       </c>
       <c r="C20" s="39" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="D20" s="39" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="E20" s="39" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="37" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="B21" s="39" t="s">
         <v>187</v>
@@ -4137,12 +4163,12 @@
         <v>187</v>
       </c>
       <c r="E21" s="39" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="37" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="B22" s="39" t="s">
         <v>187</v>
@@ -4151,15 +4177,15 @@
         <v>187</v>
       </c>
       <c r="D22" s="39" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="E22" s="39" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="40" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="B23" s="39" t="s">
         <v>39</v>
@@ -4176,7 +4202,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="40" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="B24" s="39" t="s">
         <v>39</v>
@@ -4193,41 +4219,41 @@
     </row>
     <row r="25" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="37" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="B25" s="39" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="C25" s="39" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="D25" s="39" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="E25" s="39" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="37" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="B26" s="39" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="C26" s="39" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="D26" s="39" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="E26" s="39" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="40" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="B27" s="39" t="s">
         <v>39</v>
@@ -4244,24 +4270,24 @@
     </row>
     <row r="28" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="37" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="B28" s="39" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="C28" s="39" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="D28" s="39" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="E28" s="39" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="40" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="B29" s="39" t="s">
         <v>39</v>
@@ -4278,24 +4304,24 @@
     </row>
     <row r="30" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="40" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="B30" s="39" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="C30" s="39" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="D30" s="39" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="E30" s="39" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="37" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="B31" s="39" t="s">
         <v>187</v>
@@ -4312,7 +4338,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="37" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="B32" s="39" t="s">
         <v>187</v>
@@ -4346,41 +4372,41 @@
     </row>
     <row r="34" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="37" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="B34" s="39" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="C34" s="39" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="D34" s="39" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="E34" s="39" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="37" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="B35" s="39" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="C35" s="39" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D35" s="39" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="E35" s="39" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="37" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="B36" s="39" t="s">
         <v>39</v>
@@ -4397,7 +4423,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="37" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="B37" s="39" t="s">
         <v>187</v>
@@ -4415,19 +4441,19 @@
     </row>
     <row r="38" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="37" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="B38" s="41" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="C38" s="41" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="D38" s="41" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="E38" s="41" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
     </row>
   </sheetData>
@@ -4445,32 +4471,29 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I24" activeCellId="0" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="5" style="0" width="8.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="9.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="10" style="0" width="8.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="11.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="8.63"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="42" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4478,10 +4501,10 @@
     </row>
     <row r="3" customFormat="false" ht="23.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="29" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -4492,10 +4515,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="35" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="B4" s="43" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="C4" s="43"/>
       <c r="D4" s="43"/>
@@ -4506,10 +4529,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="35" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="B5" s="43" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="C5" s="43"/>
       <c r="D5" s="43"/>
@@ -4520,10 +4543,10 @@
     </row>
     <row r="6" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="44" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -4534,10 +4557,10 @@
     </row>
     <row r="7" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="44" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="C7" s="30"/>
       <c r="D7" s="30"/>
@@ -4548,10 +4571,10 @@
     </row>
     <row r="8" customFormat="false" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="44" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="C8" s="30"/>
       <c r="D8" s="30"/>
@@ -4562,15 +4585,15 @@
     </row>
     <row r="10" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="45" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="B10" s="46" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="47" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="B11" s="47" t="n">
         <v>0.286229538687379</v>
@@ -4578,7 +4601,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="47" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="B12" s="47" t="n">
         <v>0.258073109045841</v>
@@ -4586,7 +4609,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="47" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="B13" s="47" t="n">
         <v>0.23396226376115</v>
@@ -4594,7 +4617,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="47" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="B14" s="47" t="n">
         <v>0.22173508850563</v>
@@ -4602,7 +4625,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E16" s="48" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F16" s="48"/>
       <c r="G16" s="48"/>
@@ -4610,42 +4633,42 @@
     </row>
     <row r="17" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="49" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="B17" s="49" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="C17" s="50" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="D17" s="51" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="E17" s="48" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F17" s="48" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="G17" s="48" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="H17" s="48" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="I17" s="48" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="52" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="B18" s="53" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="C18" s="54" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="D18" s="55" t="n">
         <v>0.513888888888889</v>
@@ -4654,17 +4677,18 @@
       <c r="F18" s="48"/>
       <c r="G18" s="48"/>
       <c r="H18" s="48"/>
-      <c r="I18" s="57" t="b">
+      <c r="I18" s="57" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="52"/>
       <c r="B19" s="58" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="C19" s="59" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="D19" s="60" t="n">
         <v>0.486111111111111</v>
@@ -4673,19 +4697,20 @@
       <c r="F19" s="48"/>
       <c r="G19" s="48"/>
       <c r="H19" s="48"/>
-      <c r="I19" s="61" t="b">
+      <c r="I19" s="57" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="52" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="B20" s="53" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="C20" s="54" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="D20" s="55" t="n">
         <v>0.259871031746032</v>
@@ -4694,244 +4719,254 @@
       <c r="F20" s="48"/>
       <c r="G20" s="48"/>
       <c r="H20" s="48"/>
-      <c r="I20" s="61" t="b">
+      <c r="I20" s="57" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="52"/>
-      <c r="B21" s="62" t="s">
-        <v>325</v>
+      <c r="B21" s="61" t="s">
+        <v>328</v>
       </c>
       <c r="C21" s="47" t="s">
-        <v>326</v>
-      </c>
-      <c r="D21" s="63" t="n">
+        <v>329</v>
+      </c>
+      <c r="D21" s="62" t="n">
         <v>0.238492063492063</v>
       </c>
       <c r="E21" s="56"/>
       <c r="F21" s="48"/>
       <c r="G21" s="48"/>
       <c r="H21" s="48"/>
-      <c r="I21" s="61" t="b">
+      <c r="I21" s="57" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="52"/>
-      <c r="B22" s="62" t="s">
-        <v>327</v>
+      <c r="B22" s="61" t="s">
+        <v>330</v>
       </c>
       <c r="C22" s="47" t="s">
-        <v>328</v>
-      </c>
-      <c r="D22" s="63" t="n">
+        <v>331</v>
+      </c>
+      <c r="D22" s="62" t="n">
         <v>0.246825396825397</v>
       </c>
-      <c r="E22" s="64" t="n">
+      <c r="E22" s="63" t="n">
         <v>2.75</v>
       </c>
-      <c r="F22" s="65" t="s">
+      <c r="F22" s="64" t="s">
         <v>187</v>
       </c>
-      <c r="G22" s="65" t="n">
+      <c r="G22" s="64" t="n">
         <v>1.88</v>
       </c>
-      <c r="H22" s="65" t="n">
+      <c r="H22" s="64" t="n">
         <v>3</v>
       </c>
-      <c r="I22" s="61" t="b">
+      <c r="I22" s="57" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="52"/>
       <c r="B23" s="58" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="C23" s="59" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="D23" s="60" t="n">
         <v>0.254811507936508</v>
       </c>
-      <c r="E23" s="64" t="n">
+      <c r="E23" s="63" t="n">
         <v>2.25</v>
       </c>
-      <c r="F23" s="65" t="s">
+      <c r="F23" s="64" t="s">
         <v>187</v>
       </c>
-      <c r="G23" s="65" t="n">
+      <c r="G23" s="64" t="n">
         <v>1.5</v>
       </c>
-      <c r="H23" s="65" t="n">
+      <c r="H23" s="64" t="n">
         <v>3</v>
       </c>
-      <c r="I23" s="61" t="b">
+      <c r="I23" s="57" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="66" t="s">
-        <v>331</v>
-      </c>
-      <c r="B24" s="67" t="s">
-        <v>332</v>
+      <c r="A24" s="65" t="s">
+        <v>334</v>
+      </c>
+      <c r="B24" s="66" t="s">
+        <v>335</v>
       </c>
       <c r="C24" s="47" t="s">
-        <v>333</v>
-      </c>
-      <c r="D24" s="63" t="n">
+        <v>336</v>
+      </c>
+      <c r="D24" s="62" t="n">
         <v>0.265354437229437</v>
       </c>
-      <c r="E24" s="64" t="n">
+      <c r="E24" s="63" t="n">
         <v>2</v>
       </c>
-      <c r="F24" s="65" t="s">
+      <c r="F24" s="64" t="s">
         <v>187</v>
       </c>
-      <c r="G24" s="65" t="n">
+      <c r="G24" s="64" t="n">
         <v>2.6</v>
       </c>
-      <c r="H24" s="65" t="n">
+      <c r="H24" s="64" t="n">
         <v>2.17</v>
       </c>
-      <c r="I24" s="61" t="b">
+      <c r="I24" s="57" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="N24" s="68"/>
-    </row>
-    <row r="25" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="66"/>
-      <c r="B25" s="67" t="s">
-        <v>334</v>
+      <c r="N24" s="67"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="65"/>
+      <c r="B25" s="66" t="s">
+        <v>337</v>
       </c>
       <c r="C25" s="47" t="s">
-        <v>335</v>
-      </c>
-      <c r="D25" s="63" t="n">
+        <v>338</v>
+      </c>
+      <c r="D25" s="62" t="n">
         <v>0.3964420995671</v>
       </c>
       <c r="E25" s="56"/>
       <c r="F25" s="48"/>
       <c r="G25" s="48"/>
       <c r="H25" s="48"/>
-      <c r="I25" s="61" t="b">
+      <c r="I25" s="57" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="N25" s="68"/>
-    </row>
-    <row r="26" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="66"/>
-      <c r="B26" s="69" t="s">
-        <v>336</v>
+      <c r="N25" s="67"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="65"/>
+      <c r="B26" s="68" t="s">
+        <v>339</v>
       </c>
       <c r="C26" s="59" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="D26" s="60" t="n">
         <v>0.338203463203463</v>
       </c>
-      <c r="E26" s="64" t="n">
+      <c r="E26" s="63" t="n">
         <v>2.57</v>
       </c>
-      <c r="F26" s="65" t="s">
+      <c r="F26" s="64" t="s">
         <v>187</v>
       </c>
-      <c r="G26" s="65" t="n">
+      <c r="G26" s="64" t="n">
         <v>1.71</v>
       </c>
-      <c r="H26" s="65" t="n">
+      <c r="H26" s="64" t="n">
         <v>2.14</v>
       </c>
-      <c r="I26" s="61" t="b">
+      <c r="I26" s="57" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="N26" s="68"/>
+      <c r="N26" s="67"/>
     </row>
     <row r="27" customFormat="false" ht="12.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="70" t="s">
-        <v>338</v>
-      </c>
-      <c r="B27" s="71" t="s">
-        <v>339</v>
+      <c r="A27" s="69" t="s">
+        <v>341</v>
+      </c>
+      <c r="B27" s="70" t="s">
+        <v>342</v>
       </c>
       <c r="C27" s="54" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="D27" s="55" t="n">
         <v>0.255808080808081</v>
       </c>
-      <c r="E27" s="64" t="n">
+      <c r="E27" s="63" t="n">
         <v>0</v>
       </c>
-      <c r="F27" s="65" t="s">
+      <c r="F27" s="64" t="s">
         <v>187</v>
       </c>
-      <c r="G27" s="65" t="n">
+      <c r="G27" s="64" t="n">
         <v>0.77</v>
       </c>
-      <c r="H27" s="65" t="n">
+      <c r="H27" s="64" t="n">
         <v>0.44</v>
       </c>
-      <c r="I27" s="61" t="b">
+      <c r="I27" s="57" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="J27" s="16" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="70"/>
-      <c r="B28" s="67" t="s">
-        <v>342</v>
+        <v>344</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="69"/>
+      <c r="B28" s="66" t="s">
+        <v>345</v>
       </c>
       <c r="C28" s="47" t="s">
-        <v>343</v>
-      </c>
-      <c r="D28" s="63" t="n">
+        <v>346</v>
+      </c>
+      <c r="D28" s="62" t="n">
         <v>0.383775252525253</v>
       </c>
-      <c r="E28" s="64" t="n">
+      <c r="E28" s="63" t="n">
         <v>2.63</v>
       </c>
-      <c r="F28" s="65" t="s">
+      <c r="F28" s="64" t="s">
         <v>187</v>
       </c>
-      <c r="G28" s="65" t="n">
+      <c r="G28" s="64" t="n">
         <v>1</v>
       </c>
-      <c r="H28" s="65" t="n">
+      <c r="H28" s="64" t="n">
         <v>1.88</v>
       </c>
-      <c r="I28" s="61" t="b">
+      <c r="I28" s="57" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="70"/>
-      <c r="B29" s="69" t="s">
-        <v>344</v>
+    <row r="29" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="69"/>
+      <c r="B29" s="68" t="s">
+        <v>347</v>
       </c>
       <c r="C29" s="59" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="D29" s="60" t="n">
         <v>0.360416666666667</v>
       </c>
-      <c r="E29" s="64" t="n">
+      <c r="E29" s="63" t="n">
         <v>1.63</v>
       </c>
-      <c r="F29" s="65" t="s">
+      <c r="F29" s="64" t="s">
         <v>187</v>
       </c>
-      <c r="G29" s="65" t="n">
+      <c r="G29" s="64" t="n">
         <v>1.5</v>
       </c>
-      <c r="H29" s="65" t="n">
+      <c r="H29" s="64" t="n">
         <v>2.63</v>
       </c>
-      <c r="I29" s="61" t="b">
+      <c r="I29" s="57" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
@@ -4944,16 +4979,16 @@
     </row>
     <row r="32" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="48" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="B32" s="48"/>
     </row>
     <row r="33" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="48" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="B33" s="48" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Fix computation of total demand
</commit_message>
<xml_diff>
--- a/inputs/test_input_template.xlsx
+++ b/inputs/test_input_template.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="351">
   <si>
     <t xml:space="preserve">Tool for optimizing and simulating off- and on-grid electrification solutions</t>
   </si>
@@ -901,13 +901,13 @@
     <t xml:space="preserve">default</t>
   </si>
   <si>
-    <t xml:space="preserve">critical</t>
-  </si>
-  <si>
     <t xml:space="preserve">evaluation_perspective</t>
   </si>
   <si>
     <t xml:space="preserve">AC_system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">critical_constraint</t>
   </si>
   <si>
     <t xml:space="preserve">Multicriteria analysis</t>
@@ -1726,7 +1726,7 @@
       <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="1.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.27"/>
@@ -1935,9 +1935,9 @@
       <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="18.63"/>
   </cols>
@@ -2382,11 +2382,11 @@
       <selection pane="topLeft" activeCell="A63" activeCellId="0" sqref="A63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.65234375" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="6.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="24" width="6.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="24" width="6.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="6.09"/>
   </cols>
   <sheetData>
@@ -3459,9 +3459,9 @@
       <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="20" width="12.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="20" width="12.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="20" width="9.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="20" width="6.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.36"/>
@@ -3643,8 +3643,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="20" width="8.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="20" width="9.36"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="20" min="12" style="20" width="6.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="20" width="12.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="20" width="11.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="20" width="12.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="20" width="11.11"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="23" style="20" width="6.91"/>
   </cols>
   <sheetData>
@@ -3928,10 +3928,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
+      <selection pane="topLeft" activeCell="K28" activeCellId="0" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.921875" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4392,16 +4392,16 @@
         <v>264</v>
       </c>
       <c r="B35" s="39" t="s">
-        <v>291</v>
+        <v>39</v>
       </c>
       <c r="C35" s="39" t="s">
-        <v>291</v>
+        <v>39</v>
       </c>
       <c r="D35" s="39" t="s">
-        <v>291</v>
+        <v>39</v>
       </c>
       <c r="E35" s="39" t="s">
-        <v>291</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4441,19 +4441,36 @@
     </row>
     <row r="38" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="B38" s="41" t="s">
         <v>292</v>
       </c>
-      <c r="B38" s="41" t="s">
+      <c r="C38" s="41" t="s">
+        <v>292</v>
+      </c>
+      <c r="D38" s="41" t="s">
+        <v>292</v>
+      </c>
+      <c r="E38" s="41" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="37" t="s">
         <v>293</v>
       </c>
-      <c r="C38" s="41" t="s">
-        <v>293</v>
-      </c>
-      <c r="D38" s="41" t="s">
-        <v>293</v>
-      </c>
-      <c r="E38" s="41" t="s">
-        <v>293</v>
+      <c r="B39" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="D39" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="E39" s="39" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -4481,9 +4498,9 @@
       <selection pane="topLeft" activeCell="I24" activeCellId="0" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.65234375" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.54"/>

</xml_diff>